<commit_message>
Fully integrated script now outputs the majority of important parameters for the FS design spec sheet.
</commit_message>
<xml_diff>
--- a/2020_fs_design_ic_spec_sheet_-_template.xlsx
+++ b/2020_fs_design_ic_spec_sheet_-_template.xlsx
@@ -486,12 +486,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Jounce travel in column D
-Rebound travel in column E
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Rebound travel in column E
 </t>
         </r>
       </text>
@@ -628,7 +647,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -880,13 +899,41 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Kinematic Trail
-Do not include pneumatic trail here. While not on the spec sheet, teams are expected to undertand pneumatic trail and the impact it has on vehicle dynamics.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Kinematic Trail
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Do not include pneumatic trail here. While not on the spec sheet, teams are expected to undertand pneumatic trail and the impact it has on vehicle dynamics.</t>
         </r>
       </text>
     </comment>
@@ -895,12 +942,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Front Scrub Radius</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Front Scrub Radius</t>
         </r>
       </text>
     </comment>
@@ -1125,13 +1181,41 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Steer Arm Length (mm)
-Distance from kingpin axis to center of outer tie rod.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steer Arm Length (mm)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Distance from kingpin axis to center of outer tie rod.</t>
         </r>
       </text>
     </comment>
@@ -1209,12 +1293,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">  
-Unless you have two brake pedals, the pedal Force should be the same for front and rear.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Unless you have two brake pedals, the pedal Force should be the same for front and rear.
 </t>
         </r>
       </text>
@@ -2348,7 +2441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="282">
   <si>
     <t>Car No.</t>
   </si>
@@ -3431,6 +3524,36 @@
   </si>
   <si>
     <t>Bracket and shims</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floating, 248mm diameter, 5mm cross-drilled steel		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floating, 208mm diameter, 5mm cross-drilled steel		</t>
+  </si>
+  <si>
+    <t>16.2mm bore AP Racing CP6465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilwood GP200, Aluminium, 1.25" bore		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilwood PS-1, Cast Aluminium, 1.12" bore		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machined Aluminium 6082-T6		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubber Sealed double row angular contact 3206-2RS on wheel centreline		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machined EN8 stub axle, 30mm diameter		</t>
+  </si>
+  <si>
+    <t>One-piece rotating hub-axle, machined 6082-T6 w/ 75mm diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pair of rubber sealed deep groove 61915-2RS, spaced 3mm		</t>
   </si>
 </sst>
 </file>
@@ -4264,7 +4387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4624,9 +4747,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5276,8 +5396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="131" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:H30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="131" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5291,15 +5411,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="23" x14ac:dyDescent="0.15">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="171" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
       <c r="H1" s="10">
         <v>2020</v>
       </c>
@@ -5307,56 +5427,56 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="173" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" s="13" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="194"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="193"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" s="13" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="202" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="135"/>
-      <c r="C4" s="213"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="215"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="214"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="137"/>
-      <c r="B5" s="137"/>
-      <c r="C5" s="137"/>
-      <c r="D5" s="137"/>
-      <c r="E5" s="137"/>
-      <c r="F5" s="137"/>
-      <c r="G5" s="137"/>
-      <c r="H5" s="137"/>
+      <c r="A5" s="136"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
     </row>
     <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
@@ -5365,12 +5485,12 @@
       <c r="B6" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="181"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
+      <c r="G6" s="179"/>
+      <c r="H6" s="180"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
@@ -5432,11 +5552,11 @@
       <c r="E9" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="206" t="s">
+      <c r="F9" s="205" t="s">
         <v>265</v>
       </c>
-      <c r="G9" s="198"/>
-      <c r="H9" s="199"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="198"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
@@ -5475,17 +5595,17 @@
       <c r="F11" s="90">
         <v>50</v>
       </c>
-      <c r="G11" s="195"/>
-      <c r="H11" s="196"/>
+      <c r="G11" s="194"/>
+      <c r="H11" s="195"/>
     </row>
     <row r="12" spans="1:10" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="137"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="E12" s="137"/>
-      <c r="F12" s="137"/>
-      <c r="G12" s="137"/>
-      <c r="H12" s="137"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="136"/>
+      <c r="H12" s="136"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
@@ -5494,28 +5614,28 @@
       <c r="B13" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="182" t="s">
+      <c r="C13" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="183"/>
-      <c r="E13" s="184"/>
-      <c r="F13" s="185" t="s">
+      <c r="D13" s="182"/>
+      <c r="E13" s="183"/>
+      <c r="F13" s="184" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="183"/>
-      <c r="H13" s="184"/>
+      <c r="G13" s="182"/>
+      <c r="H13" s="183"/>
     </row>
     <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
         <v>235</v>
       </c>
       <c r="B14" s="64"/>
-      <c r="C14" s="216" t="s">
+      <c r="C14" s="215" t="s">
         <v>261</v>
       </c>
       <c r="D14" s="84"/>
       <c r="E14" s="87"/>
-      <c r="F14" s="216" t="s">
+      <c r="F14" s="215" t="s">
         <v>261</v>
       </c>
       <c r="G14" s="84"/>
@@ -5528,48 +5648,48 @@
       <c r="B15" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="207" t="s">
+      <c r="C15" s="206" t="s">
         <v>262</v>
       </c>
-      <c r="D15" s="208"/>
-      <c r="E15" s="209"/>
-      <c r="F15" s="207" t="s">
+      <c r="D15" s="207"/>
+      <c r="E15" s="208"/>
+      <c r="F15" s="206" t="s">
         <v>262</v>
       </c>
-      <c r="G15" s="208"/>
-      <c r="H15" s="209"/>
+      <c r="G15" s="207"/>
+      <c r="H15" s="208"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="20" t="s">
         <v>200</v>
       </c>
       <c r="B16" s="64"/>
-      <c r="C16" s="207" t="s">
+      <c r="C16" s="206" t="s">
         <v>263</v>
       </c>
-      <c r="D16" s="208"/>
-      <c r="E16" s="209"/>
-      <c r="F16" s="207" t="s">
+      <c r="D16" s="207"/>
+      <c r="E16" s="208"/>
+      <c r="F16" s="206" t="s">
         <v>263</v>
       </c>
-      <c r="G16" s="208"/>
-      <c r="H16" s="209"/>
+      <c r="G16" s="207"/>
+      <c r="H16" s="208"/>
     </row>
     <row r="17" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="64"/>
-      <c r="C17" s="204" t="s">
+      <c r="C17" s="203" t="s">
         <v>264</v>
       </c>
-      <c r="D17" s="198"/>
-      <c r="E17" s="199"/>
-      <c r="F17" s="205" t="s">
+      <c r="D17" s="197"/>
+      <c r="E17" s="198"/>
+      <c r="F17" s="204" t="s">
         <v>264</v>
       </c>
-      <c r="G17" s="198"/>
-      <c r="H17" s="199"/>
+      <c r="G17" s="197"/>
+      <c r="H17" s="198"/>
     </row>
     <row r="18" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="20" t="s">
@@ -5578,7 +5698,7 @@
       <c r="B18" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="121" t="s">
         <v>147</v>
       </c>
       <c r="D18" s="102">
@@ -5587,7 +5707,7 @@
       <c r="E18" s="95">
         <v>30</v>
       </c>
-      <c r="F18" s="123" t="s">
+      <c r="F18" s="122" t="s">
         <v>148</v>
       </c>
       <c r="G18" s="94">
@@ -5605,11 +5725,11 @@
         <v>70</v>
       </c>
       <c r="C19" s="96"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="133"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="132"/>
       <c r="F19" s="97"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="133"/>
+      <c r="G19" s="131"/>
+      <c r="H19" s="132"/>
     </row>
     <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="20" t="s">
@@ -5618,11 +5738,11 @@
       <c r="B20" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="D20" s="132"/>
-      <c r="E20" s="133"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="132"/>
       <c r="F20" s="97"/>
-      <c r="G20" s="132"/>
-      <c r="H20" s="133"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="132"/>
     </row>
     <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
@@ -5632,11 +5752,11 @@
         <v>71</v>
       </c>
       <c r="C21" s="98"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="133"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="132"/>
       <c r="F21" s="99"/>
-      <c r="G21" s="132"/>
-      <c r="H21" s="133"/>
+      <c r="G21" s="131"/>
+      <c r="H21" s="132"/>
     </row>
     <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
@@ -5705,12 +5825,14 @@
       <c r="B25" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="113"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="133"/>
+      <c r="C25" s="113">
+        <v>47.8</v>
+      </c>
+      <c r="D25" s="131"/>
+      <c r="E25" s="132"/>
       <c r="F25" s="38"/>
-      <c r="G25" s="132"/>
-      <c r="H25" s="133"/>
+      <c r="G25" s="131"/>
+      <c r="H25" s="132"/>
     </row>
     <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="20" t="s">
@@ -5719,12 +5841,14 @@
       <c r="B26" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="113"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="133"/>
+      <c r="C26" s="113">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="D26" s="131"/>
+      <c r="E26" s="132"/>
       <c r="F26" s="38"/>
-      <c r="G26" s="132"/>
-      <c r="H26" s="133"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="132"/>
     </row>
     <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="20" t="s">
@@ -5733,12 +5857,16 @@
       <c r="B27" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="100"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="133"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="132"/>
-      <c r="H27" s="133"/>
+      <c r="C27" s="100">
+        <v>0</v>
+      </c>
+      <c r="D27" s="131"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="G27" s="131"/>
+      <c r="H27" s="132"/>
     </row>
     <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="20" t="s">
@@ -5750,29 +5878,29 @@
       <c r="C28" s="100">
         <v>-1.5</v>
       </c>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="132"/>
       <c r="F28" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="G28" s="132"/>
-      <c r="H28" s="133"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="132"/>
     </row>
     <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="20" t="s">
         <v>95</v>
       </c>
       <c r="B29" s="64"/>
-      <c r="C29" s="189" t="s">
+      <c r="C29" s="188" t="s">
         <v>267</v>
       </c>
-      <c r="D29" s="140"/>
-      <c r="E29" s="141"/>
-      <c r="F29" s="212" t="s">
+      <c r="D29" s="139"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="211" t="s">
         <v>267</v>
       </c>
-      <c r="G29" s="140"/>
-      <c r="H29" s="141"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="140"/>
     </row>
     <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="20" t="s">
@@ -5784,13 +5912,13 @@
       <c r="C30" s="112">
         <v>0</v>
       </c>
-      <c r="D30" s="132"/>
-      <c r="E30" s="133"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="132"/>
       <c r="F30" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="G30" s="132"/>
-      <c r="H30" s="133"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="132"/>
     </row>
     <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="20" t="s">
@@ -5802,13 +5930,13 @@
       <c r="C31" s="113">
         <v>29.2</v>
       </c>
-      <c r="D31" s="132"/>
-      <c r="E31" s="133"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
       <c r="F31" s="114">
         <v>37.1</v>
       </c>
-      <c r="G31" s="132"/>
-      <c r="H31" s="133"/>
+      <c r="G31" s="131"/>
+      <c r="H31" s="132"/>
     </row>
     <row r="32" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
@@ -5817,12 +5945,12 @@
       <c r="B32" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="122" t="s">
+      <c r="C32" s="121" t="s">
         <v>198</v>
       </c>
       <c r="D32" s="102"/>
       <c r="E32" s="95"/>
-      <c r="F32" s="123" t="s">
+      <c r="F32" s="122" t="s">
         <v>199</v>
       </c>
       <c r="G32" s="94"/>
@@ -5836,11 +5964,15 @@
       <c r="C33" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="115"/>
+      <c r="D33" s="115">
+        <v>4.7</v>
+      </c>
       <c r="E33" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="F33" s="116"/>
+      <c r="F33" s="116">
+        <v>20.8</v>
+      </c>
       <c r="G33" s="74" t="s">
         <v>180</v>
       </c>
@@ -5856,13 +5988,17 @@
       <c r="C34" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="108"/>
+      <c r="D34" s="108">
+        <v>9.5</v>
+      </c>
       <c r="E34" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="108"/>
-      <c r="G34" s="210"/>
-      <c r="H34" s="211"/>
+      <c r="F34" s="108">
+        <v>53.7</v>
+      </c>
+      <c r="G34" s="209"/>
+      <c r="H34" s="210"/>
     </row>
     <row r="35" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="20" t="s">
@@ -5880,23 +6016,23 @@
       <c r="E35" s="39" t="s">
         <v>270</v>
       </c>
-      <c r="F35" s="186"/>
-      <c r="G35" s="187"/>
-      <c r="H35" s="188"/>
+      <c r="F35" s="185"/>
+      <c r="G35" s="186"/>
+      <c r="H35" s="187"/>
     </row>
     <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="22" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="65"/>
-      <c r="C36" s="197" t="s">
+      <c r="C36" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="D36" s="198"/>
-      <c r="E36" s="198"/>
-      <c r="F36" s="198"/>
-      <c r="G36" s="198"/>
-      <c r="H36" s="199"/>
+      <c r="D36" s="197"/>
+      <c r="E36" s="197"/>
+      <c r="F36" s="197"/>
+      <c r="G36" s="197"/>
+      <c r="H36" s="198"/>
     </row>
     <row r="37" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
@@ -5919,14 +6055,14 @@
       <c r="H37" s="120"/>
     </row>
     <row r="38" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="137"/>
-      <c r="B38" s="137"/>
-      <c r="C38" s="137"/>
-      <c r="D38" s="137"/>
-      <c r="E38" s="137"/>
-      <c r="F38" s="137"/>
-      <c r="G38" s="137"/>
-      <c r="H38" s="137"/>
+      <c r="A38" s="136"/>
+      <c r="B38" s="136"/>
+      <c r="C38" s="136"/>
+      <c r="D38" s="136"/>
+      <c r="E38" s="136"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="136"/>
+      <c r="H38" s="136"/>
     </row>
     <row r="39" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="19" t="s">
@@ -5935,64 +6071,76 @@
       <c r="B39" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="182" t="s">
+      <c r="C39" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
-      <c r="F39" s="182" t="s">
+      <c r="D39" s="182"/>
+      <c r="E39" s="183"/>
+      <c r="F39" s="181" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="183"/>
-      <c r="H39" s="184"/>
+      <c r="G39" s="182"/>
+      <c r="H39" s="183"/>
     </row>
     <row r="40" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="40"/>
-      <c r="C40" s="139"/>
-      <c r="D40" s="140"/>
-      <c r="E40" s="141"/>
-      <c r="F40" s="139"/>
-      <c r="G40" s="140"/>
-      <c r="H40" s="141"/>
+      <c r="C40" s="138" t="s">
+        <v>272</v>
+      </c>
+      <c r="D40" s="139"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="138" t="s">
+        <v>273</v>
+      </c>
+      <c r="G40" s="139"/>
+      <c r="H40" s="140"/>
     </row>
     <row r="41" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="40"/>
-      <c r="C41" s="139"/>
-      <c r="D41" s="140"/>
-      <c r="E41" s="141"/>
-      <c r="F41" s="139"/>
-      <c r="G41" s="140"/>
-      <c r="H41" s="141"/>
+      <c r="C41" s="138" t="s">
+        <v>274</v>
+      </c>
+      <c r="D41" s="139"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="138" t="s">
+        <v>274</v>
+      </c>
+      <c r="G41" s="139"/>
+      <c r="H41" s="140"/>
     </row>
     <row r="42" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="40"/>
-      <c r="C42" s="139"/>
-      <c r="D42" s="140"/>
-      <c r="E42" s="141"/>
-      <c r="F42" s="139"/>
-      <c r="G42" s="140"/>
-      <c r="H42" s="141"/>
+      <c r="C42" s="138" t="s">
+        <v>275</v>
+      </c>
+      <c r="D42" s="139"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="138" t="s">
+        <v>276</v>
+      </c>
+      <c r="G42" s="139"/>
+      <c r="H42" s="140"/>
     </row>
     <row r="43" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="20" t="s">
         <v>179</v>
       </c>
       <c r="B43" s="40"/>
-      <c r="C43" s="139"/>
-      <c r="D43" s="140"/>
-      <c r="E43" s="141"/>
-      <c r="F43" s="139"/>
-      <c r="G43" s="140"/>
-      <c r="H43" s="141"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="140"/>
+      <c r="F43" s="138"/>
+      <c r="G43" s="139"/>
+      <c r="H43" s="140"/>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="20" t="s">
@@ -6002,61 +6150,79 @@
       <c r="C44" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="121"/>
+      <c r="D44" s="215">
+        <v>25.1</v>
+      </c>
       <c r="E44" s="56" t="s">
         <v>168</v>
       </c>
-      <c r="F44" s="108"/>
+      <c r="F44" s="215">
+        <v>25.1</v>
+      </c>
       <c r="G44" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="H44" s="104"/>
+      <c r="H44" s="215">
+        <v>425</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B45" s="41"/>
-      <c r="C45" s="139"/>
-      <c r="D45" s="140"/>
-      <c r="E45" s="141"/>
-      <c r="F45" s="139"/>
-      <c r="G45" s="140"/>
-      <c r="H45" s="141"/>
+      <c r="C45" s="138" t="s">
+        <v>277</v>
+      </c>
+      <c r="D45" s="139"/>
+      <c r="E45" s="140"/>
+      <c r="F45" s="138" t="s">
+        <v>277</v>
+      </c>
+      <c r="G45" s="139"/>
+      <c r="H45" s="140"/>
     </row>
     <row r="46" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="40"/>
-      <c r="C46" s="139"/>
-      <c r="D46" s="140"/>
-      <c r="E46" s="141"/>
-      <c r="F46" s="139"/>
-      <c r="G46" s="140"/>
-      <c r="H46" s="141"/>
+      <c r="C46" s="138" t="s">
+        <v>278</v>
+      </c>
+      <c r="D46" s="139"/>
+      <c r="E46" s="140"/>
+      <c r="F46" s="138" t="s">
+        <v>281</v>
+      </c>
+      <c r="G46" s="139"/>
+      <c r="H46" s="140"/>
     </row>
     <row r="47" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="42"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="136"/>
-      <c r="F47" s="138"/>
-      <c r="G47" s="135"/>
-      <c r="H47" s="136"/>
+      <c r="C47" s="137" t="s">
+        <v>279</v>
+      </c>
+      <c r="D47" s="134"/>
+      <c r="E47" s="135"/>
+      <c r="F47" s="137" t="s">
+        <v>280</v>
+      </c>
+      <c r="G47" s="134"/>
+      <c r="H47" s="135"/>
     </row>
     <row r="48" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="137"/>
-      <c r="B48" s="137"/>
-      <c r="C48" s="137"/>
-      <c r="D48" s="137"/>
-      <c r="E48" s="137"/>
-      <c r="F48" s="137"/>
-      <c r="G48" s="137"/>
-      <c r="H48" s="137"/>
+      <c r="A48" s="136"/>
+      <c r="B48" s="136"/>
+      <c r="C48" s="136"/>
+      <c r="D48" s="136"/>
+      <c r="E48" s="136"/>
+      <c r="F48" s="136"/>
+      <c r="G48" s="136"/>
+      <c r="H48" s="136"/>
     </row>
     <row r="49" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="19" t="s">
@@ -6065,36 +6231,36 @@
       <c r="B49" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="145"/>
-      <c r="D49" s="146"/>
-      <c r="E49" s="146"/>
-      <c r="F49" s="146"/>
-      <c r="G49" s="146"/>
-      <c r="H49" s="147"/>
+      <c r="C49" s="144"/>
+      <c r="D49" s="145"/>
+      <c r="E49" s="145"/>
+      <c r="F49" s="145"/>
+      <c r="G49" s="145"/>
+      <c r="H49" s="146"/>
     </row>
     <row r="50" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="30"/>
-      <c r="C50" s="128"/>
-      <c r="D50" s="129"/>
-      <c r="E50" s="129"/>
-      <c r="F50" s="129"/>
-      <c r="G50" s="129"/>
-      <c r="H50" s="130"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="128"/>
+      <c r="E50" s="128"/>
+      <c r="F50" s="128"/>
+      <c r="G50" s="128"/>
+      <c r="H50" s="129"/>
     </row>
     <row r="51" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="30"/>
-      <c r="C51" s="128"/>
-      <c r="D51" s="129"/>
-      <c r="E51" s="129"/>
-      <c r="F51" s="129"/>
-      <c r="G51" s="129"/>
-      <c r="H51" s="130"/>
+      <c r="C51" s="127"/>
+      <c r="D51" s="128"/>
+      <c r="E51" s="128"/>
+      <c r="F51" s="128"/>
+      <c r="G51" s="128"/>
+      <c r="H51" s="129"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="20" t="s">
@@ -6108,77 +6274,77 @@
       <c r="E52" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="F52" s="200"/>
-      <c r="G52" s="201"/>
-      <c r="H52" s="202"/>
+      <c r="F52" s="199"/>
+      <c r="G52" s="200"/>
+      <c r="H52" s="201"/>
     </row>
     <row r="53" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="30"/>
-      <c r="C53" s="128"/>
-      <c r="D53" s="129"/>
-      <c r="E53" s="129"/>
-      <c r="F53" s="129"/>
-      <c r="G53" s="129"/>
-      <c r="H53" s="130"/>
+      <c r="C53" s="127"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="128"/>
+      <c r="F53" s="128"/>
+      <c r="G53" s="128"/>
+      <c r="H53" s="129"/>
     </row>
     <row r="54" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B54" s="30"/>
-      <c r="C54" s="128"/>
-      <c r="D54" s="129"/>
-      <c r="E54" s="129"/>
-      <c r="F54" s="129"/>
-      <c r="G54" s="129"/>
-      <c r="H54" s="130"/>
+      <c r="C54" s="127"/>
+      <c r="D54" s="128"/>
+      <c r="E54" s="128"/>
+      <c r="F54" s="128"/>
+      <c r="G54" s="128"/>
+      <c r="H54" s="129"/>
     </row>
     <row r="55" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B55" s="30"/>
-      <c r="C55" s="128"/>
-      <c r="D55" s="129"/>
-      <c r="E55" s="129"/>
-      <c r="F55" s="129"/>
-      <c r="G55" s="129"/>
-      <c r="H55" s="130"/>
+      <c r="C55" s="127"/>
+      <c r="D55" s="128"/>
+      <c r="E55" s="128"/>
+      <c r="F55" s="128"/>
+      <c r="G55" s="128"/>
+      <c r="H55" s="129"/>
     </row>
     <row r="56" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="79" t="s">
         <v>178</v>
       </c>
       <c r="B56" s="80"/>
-      <c r="C56" s="176"/>
-      <c r="D56" s="177"/>
-      <c r="E56" s="177"/>
-      <c r="F56" s="177"/>
-      <c r="G56" s="177"/>
-      <c r="H56" s="178"/>
+      <c r="C56" s="175"/>
+      <c r="D56" s="176"/>
+      <c r="E56" s="176"/>
+      <c r="F56" s="176"/>
+      <c r="G56" s="176"/>
+      <c r="H56" s="177"/>
     </row>
     <row r="57" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="131"/>
-      <c r="B57" s="131"/>
-      <c r="C57" s="131"/>
-      <c r="D57" s="131"/>
-      <c r="E57" s="131"/>
-      <c r="F57" s="131"/>
-      <c r="G57" s="131"/>
-      <c r="H57" s="131"/>
+      <c r="A57" s="130"/>
+      <c r="B57" s="130"/>
+      <c r="C57" s="130"/>
+      <c r="D57" s="130"/>
+      <c r="E57" s="130"/>
+      <c r="F57" s="130"/>
+      <c r="G57" s="130"/>
+      <c r="H57" s="130"/>
     </row>
     <row r="58" spans="1:8" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="127"/>
-      <c r="B58" s="127"/>
-      <c r="C58" s="127"/>
-      <c r="D58" s="127"/>
-      <c r="E58" s="127"/>
-      <c r="F58" s="127"/>
-      <c r="G58" s="127"/>
-      <c r="H58" s="127"/>
+      <c r="A58" s="126"/>
+      <c r="B58" s="126"/>
+      <c r="C58" s="126"/>
+      <c r="D58" s="126"/>
+      <c r="E58" s="126"/>
+      <c r="F58" s="126"/>
+      <c r="G58" s="126"/>
+      <c r="H58" s="126"/>
     </row>
     <row r="59" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="19" t="s">
@@ -6187,106 +6353,106 @@
       <c r="B59" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="145"/>
-      <c r="D59" s="146"/>
-      <c r="E59" s="146"/>
-      <c r="F59" s="146"/>
-      <c r="G59" s="146"/>
-      <c r="H59" s="147"/>
+      <c r="C59" s="144"/>
+      <c r="D59" s="145"/>
+      <c r="E59" s="145"/>
+      <c r="F59" s="145"/>
+      <c r="G59" s="145"/>
+      <c r="H59" s="146"/>
     </row>
     <row r="60" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="20" t="s">
         <v>175</v>
       </c>
       <c r="B60" s="31"/>
-      <c r="C60" s="128"/>
-      <c r="D60" s="129"/>
-      <c r="E60" s="129"/>
-      <c r="F60" s="129"/>
-      <c r="G60" s="129"/>
-      <c r="H60" s="130"/>
+      <c r="C60" s="127"/>
+      <c r="D60" s="128"/>
+      <c r="E60" s="128"/>
+      <c r="F60" s="128"/>
+      <c r="G60" s="128"/>
+      <c r="H60" s="129"/>
     </row>
     <row r="61" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="31"/>
-      <c r="C61" s="128"/>
-      <c r="D61" s="129"/>
-      <c r="E61" s="129"/>
-      <c r="F61" s="129"/>
-      <c r="G61" s="129"/>
-      <c r="H61" s="130"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="128"/>
+      <c r="E61" s="128"/>
+      <c r="F61" s="128"/>
+      <c r="G61" s="128"/>
+      <c r="H61" s="129"/>
     </row>
     <row r="62" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="20" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="31"/>
-      <c r="C62" s="128"/>
-      <c r="D62" s="129"/>
-      <c r="E62" s="129"/>
-      <c r="F62" s="129"/>
-      <c r="G62" s="129"/>
-      <c r="H62" s="130"/>
+      <c r="C62" s="127"/>
+      <c r="D62" s="128"/>
+      <c r="E62" s="128"/>
+      <c r="F62" s="128"/>
+      <c r="G62" s="128"/>
+      <c r="H62" s="129"/>
     </row>
     <row r="63" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B63" s="30"/>
-      <c r="C63" s="128"/>
-      <c r="D63" s="129"/>
-      <c r="E63" s="129"/>
-      <c r="F63" s="129"/>
-      <c r="G63" s="129"/>
-      <c r="H63" s="130"/>
+      <c r="C63" s="127"/>
+      <c r="D63" s="128"/>
+      <c r="E63" s="128"/>
+      <c r="F63" s="128"/>
+      <c r="G63" s="128"/>
+      <c r="H63" s="129"/>
     </row>
     <row r="64" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="20" t="s">
         <v>51</v>
       </c>
       <c r="B64" s="31"/>
-      <c r="C64" s="128"/>
-      <c r="D64" s="129"/>
-      <c r="E64" s="129"/>
-      <c r="F64" s="129"/>
-      <c r="G64" s="129"/>
-      <c r="H64" s="130"/>
+      <c r="C64" s="127"/>
+      <c r="D64" s="128"/>
+      <c r="E64" s="128"/>
+      <c r="F64" s="128"/>
+      <c r="G64" s="128"/>
+      <c r="H64" s="129"/>
     </row>
     <row r="65" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="20" t="s">
         <v>55</v>
       </c>
       <c r="B65" s="31"/>
-      <c r="C65" s="128"/>
-      <c r="D65" s="129"/>
-      <c r="E65" s="129"/>
-      <c r="F65" s="129"/>
-      <c r="G65" s="129"/>
-      <c r="H65" s="130"/>
+      <c r="C65" s="127"/>
+      <c r="D65" s="128"/>
+      <c r="E65" s="128"/>
+      <c r="F65" s="128"/>
+      <c r="G65" s="128"/>
+      <c r="H65" s="129"/>
     </row>
     <row r="66" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B66" s="32"/>
-      <c r="C66" s="155"/>
-      <c r="D66" s="156"/>
-      <c r="E66" s="156"/>
-      <c r="F66" s="156"/>
-      <c r="G66" s="156"/>
-      <c r="H66" s="157"/>
+      <c r="C66" s="154"/>
+      <c r="D66" s="155"/>
+      <c r="E66" s="155"/>
+      <c r="F66" s="155"/>
+      <c r="G66" s="155"/>
+      <c r="H66" s="156"/>
     </row>
     <row r="67" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="137"/>
-      <c r="B67" s="137"/>
-      <c r="C67" s="137"/>
-      <c r="D67" s="137"/>
-      <c r="E67" s="137"/>
-      <c r="F67" s="137"/>
-      <c r="G67" s="137"/>
-      <c r="H67" s="137"/>
+      <c r="A67" s="136"/>
+      <c r="B67" s="136"/>
+      <c r="C67" s="136"/>
+      <c r="D67" s="136"/>
+      <c r="E67" s="136"/>
+      <c r="F67" s="136"/>
+      <c r="G67" s="136"/>
+      <c r="H67" s="136"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="19" t="s">
@@ -6295,48 +6461,48 @@
       <c r="B68" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C68" s="145"/>
-      <c r="D68" s="146"/>
-      <c r="E68" s="146"/>
-      <c r="F68" s="146"/>
-      <c r="G68" s="146"/>
-      <c r="H68" s="147"/>
+      <c r="C68" s="144"/>
+      <c r="D68" s="145"/>
+      <c r="E68" s="145"/>
+      <c r="F68" s="145"/>
+      <c r="G68" s="145"/>
+      <c r="H68" s="146"/>
     </row>
     <row r="69" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B69" s="67"/>
-      <c r="C69" s="128"/>
-      <c r="D69" s="129"/>
-      <c r="E69" s="129"/>
-      <c r="F69" s="129"/>
-      <c r="G69" s="129"/>
-      <c r="H69" s="130"/>
+      <c r="C69" s="127"/>
+      <c r="D69" s="128"/>
+      <c r="E69" s="128"/>
+      <c r="F69" s="128"/>
+      <c r="G69" s="128"/>
+      <c r="H69" s="129"/>
     </row>
     <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B70" s="67"/>
-      <c r="C70" s="128"/>
-      <c r="D70" s="129"/>
-      <c r="E70" s="129"/>
-      <c r="F70" s="129"/>
-      <c r="G70" s="129"/>
-      <c r="H70" s="130"/>
+      <c r="C70" s="127"/>
+      <c r="D70" s="128"/>
+      <c r="E70" s="128"/>
+      <c r="F70" s="128"/>
+      <c r="G70" s="128"/>
+      <c r="H70" s="129"/>
     </row>
     <row r="71" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B71" s="67"/>
-      <c r="C71" s="128"/>
-      <c r="D71" s="129"/>
-      <c r="E71" s="129"/>
-      <c r="F71" s="129"/>
-      <c r="G71" s="129"/>
-      <c r="H71" s="130"/>
+      <c r="C71" s="127"/>
+      <c r="D71" s="128"/>
+      <c r="E71" s="128"/>
+      <c r="F71" s="128"/>
+      <c r="G71" s="128"/>
+      <c r="H71" s="129"/>
     </row>
     <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="23" t="s">
@@ -6353,8 +6519,8 @@
         <v>108</v>
       </c>
       <c r="F72" s="108"/>
-      <c r="G72" s="132"/>
-      <c r="H72" s="133"/>
+      <c r="G72" s="131"/>
+      <c r="H72" s="132"/>
     </row>
     <row r="73" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="23" t="s">
@@ -6381,24 +6547,24 @@
         <v>104</v>
       </c>
       <c r="B74" s="67"/>
-      <c r="C74" s="128"/>
-      <c r="D74" s="129"/>
-      <c r="E74" s="129"/>
-      <c r="F74" s="129"/>
-      <c r="G74" s="129"/>
-      <c r="H74" s="130"/>
+      <c r="C74" s="127"/>
+      <c r="D74" s="128"/>
+      <c r="E74" s="128"/>
+      <c r="F74" s="128"/>
+      <c r="G74" s="128"/>
+      <c r="H74" s="129"/>
     </row>
     <row r="75" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="23" t="s">
         <v>167</v>
       </c>
       <c r="B75" s="67"/>
-      <c r="C75" s="128"/>
-      <c r="D75" s="129"/>
-      <c r="E75" s="129"/>
-      <c r="F75" s="129"/>
-      <c r="G75" s="129"/>
-      <c r="H75" s="130"/>
+      <c r="C75" s="127"/>
+      <c r="D75" s="128"/>
+      <c r="E75" s="128"/>
+      <c r="F75" s="128"/>
+      <c r="G75" s="128"/>
+      <c r="H75" s="129"/>
     </row>
     <row r="76" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="23" t="s">
@@ -6434,19 +6600,19 @@
       <c r="E77" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" s="134"/>
-      <c r="G77" s="135"/>
-      <c r="H77" s="136"/>
+      <c r="F77" s="133"/>
+      <c r="G77" s="134"/>
+      <c r="H77" s="135"/>
     </row>
     <row r="78" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="158"/>
-      <c r="B78" s="158"/>
-      <c r="C78" s="158"/>
-      <c r="D78" s="158"/>
-      <c r="E78" s="158"/>
-      <c r="F78" s="158"/>
-      <c r="G78" s="158"/>
-      <c r="H78" s="158"/>
+      <c r="A78" s="157"/>
+      <c r="B78" s="157"/>
+      <c r="C78" s="157"/>
+      <c r="D78" s="157"/>
+      <c r="E78" s="157"/>
+      <c r="F78" s="157"/>
+      <c r="G78" s="157"/>
+      <c r="H78" s="157"/>
     </row>
     <row r="79" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="25" t="s">
@@ -6455,39 +6621,39 @@
       <c r="B79" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="145"/>
-      <c r="D79" s="146"/>
-      <c r="E79" s="146"/>
-      <c r="F79" s="146"/>
-      <c r="G79" s="146"/>
-      <c r="H79" s="147"/>
+      <c r="C79" s="144"/>
+      <c r="D79" s="145"/>
+      <c r="E79" s="145"/>
+      <c r="F79" s="145"/>
+      <c r="G79" s="145"/>
+      <c r="H79" s="146"/>
     </row>
     <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B80" s="67"/>
-      <c r="C80" s="139"/>
-      <c r="D80" s="140"/>
-      <c r="E80" s="140"/>
-      <c r="F80" s="140"/>
-      <c r="G80" s="140"/>
-      <c r="H80" s="141"/>
+      <c r="C80" s="138"/>
+      <c r="D80" s="139"/>
+      <c r="E80" s="139"/>
+      <c r="F80" s="139"/>
+      <c r="G80" s="139"/>
+      <c r="H80" s="140"/>
     </row>
     <row r="81" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="23" t="s">
         <v>116</v>
       </c>
       <c r="B81" s="67"/>
-      <c r="C81" s="151" t="s">
+      <c r="C81" s="150" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="152"/>
+      <c r="D81" s="151"/>
       <c r="E81" s="91"/>
-      <c r="F81" s="153" t="s">
+      <c r="F81" s="152" t="s">
         <v>172</v>
       </c>
-      <c r="G81" s="154"/>
+      <c r="G81" s="153"/>
       <c r="H81" s="48"/>
     </row>
     <row r="82" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -6495,15 +6661,15 @@
         <v>115</v>
       </c>
       <c r="B82" s="67"/>
-      <c r="C82" s="151" t="s">
+      <c r="C82" s="150" t="s">
         <v>112</v>
       </c>
-      <c r="D82" s="152"/>
+      <c r="D82" s="151"/>
       <c r="E82" s="91"/>
-      <c r="F82" s="153" t="s">
+      <c r="F82" s="152" t="s">
         <v>113</v>
       </c>
-      <c r="G82" s="154"/>
+      <c r="G82" s="153"/>
       <c r="H82" s="95"/>
     </row>
     <row r="83" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -6513,15 +6679,15 @@
       <c r="B83" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="151" t="s">
+      <c r="C83" s="150" t="s">
         <v>153</v>
       </c>
-      <c r="D83" s="152"/>
+      <c r="D83" s="151"/>
       <c r="E83" s="102"/>
-      <c r="F83" s="153">
+      <c r="F83" s="152">
         <v>84.5</v>
       </c>
-      <c r="G83" s="154"/>
+      <c r="G83" s="153"/>
       <c r="H83" s="95"/>
     </row>
     <row r="84" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -6537,8 +6703,8 @@
         <v>164</v>
       </c>
       <c r="F84" s="17"/>
-      <c r="G84" s="170"/>
-      <c r="H84" s="171"/>
+      <c r="G84" s="169"/>
+      <c r="H84" s="170"/>
     </row>
     <row r="85" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="23" t="s">
@@ -6565,48 +6731,48 @@
         <v>48</v>
       </c>
       <c r="B86" s="67"/>
-      <c r="C86" s="139"/>
-      <c r="D86" s="140"/>
-      <c r="E86" s="140"/>
-      <c r="F86" s="140"/>
-      <c r="G86" s="140"/>
-      <c r="H86" s="141"/>
+      <c r="C86" s="138"/>
+      <c r="D86" s="139"/>
+      <c r="E86" s="139"/>
+      <c r="F86" s="139"/>
+      <c r="G86" s="139"/>
+      <c r="H86" s="140"/>
     </row>
     <row r="87" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="23" t="s">
         <v>46</v>
       </c>
       <c r="B87" s="67"/>
-      <c r="C87" s="139"/>
-      <c r="D87" s="140"/>
-      <c r="E87" s="140"/>
-      <c r="F87" s="140"/>
-      <c r="G87" s="140"/>
-      <c r="H87" s="141"/>
+      <c r="C87" s="138"/>
+      <c r="D87" s="139"/>
+      <c r="E87" s="139"/>
+      <c r="F87" s="139"/>
+      <c r="G87" s="139"/>
+      <c r="H87" s="140"/>
     </row>
     <row r="88" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B88" s="67"/>
-      <c r="C88" s="139"/>
-      <c r="D88" s="140"/>
-      <c r="E88" s="140"/>
-      <c r="F88" s="140"/>
-      <c r="G88" s="140"/>
-      <c r="H88" s="141"/>
+      <c r="C88" s="138"/>
+      <c r="D88" s="139"/>
+      <c r="E88" s="139"/>
+      <c r="F88" s="139"/>
+      <c r="G88" s="139"/>
+      <c r="H88" s="140"/>
     </row>
     <row r="89" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="23" t="s">
         <v>123</v>
       </c>
       <c r="B89" s="67"/>
-      <c r="C89" s="139"/>
-      <c r="D89" s="140"/>
-      <c r="E89" s="140"/>
-      <c r="F89" s="140"/>
-      <c r="G89" s="140"/>
-      <c r="H89" s="141"/>
+      <c r="C89" s="138"/>
+      <c r="D89" s="139"/>
+      <c r="E89" s="139"/>
+      <c r="F89" s="139"/>
+      <c r="G89" s="139"/>
+      <c r="H89" s="140"/>
     </row>
     <row r="90" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="23" t="s">
@@ -6616,25 +6782,25 @@
         <v>80</v>
       </c>
       <c r="C90" s="44"/>
-      <c r="D90" s="165"/>
-      <c r="E90" s="166"/>
-      <c r="F90" s="166"/>
-      <c r="G90" s="166"/>
-      <c r="H90" s="167"/>
+      <c r="D90" s="164"/>
+      <c r="E90" s="165"/>
+      <c r="F90" s="165"/>
+      <c r="G90" s="165"/>
+      <c r="H90" s="166"/>
     </row>
     <row r="91" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B91" s="67"/>
-      <c r="C91" s="139" t="s">
+      <c r="C91" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="D91" s="140"/>
-      <c r="E91" s="140"/>
-      <c r="F91" s="140"/>
-      <c r="G91" s="140"/>
-      <c r="H91" s="141"/>
+      <c r="D91" s="139"/>
+      <c r="E91" s="139"/>
+      <c r="F91" s="139"/>
+      <c r="G91" s="139"/>
+      <c r="H91" s="140"/>
     </row>
     <row r="92" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="23" t="s">
@@ -6645,10 +6811,10 @@
         <v>121</v>
       </c>
       <c r="D92" s="109"/>
-      <c r="E92" s="160" t="s">
+      <c r="E92" s="159" t="s">
         <v>120</v>
       </c>
-      <c r="F92" s="161"/>
+      <c r="F92" s="160"/>
       <c r="G92" s="94"/>
       <c r="H92" s="50"/>
     </row>
@@ -6658,10 +6824,10 @@
       </c>
       <c r="B93" s="67"/>
       <c r="C93" s="44"/>
-      <c r="D93" s="168" t="s">
+      <c r="D93" s="167" t="s">
         <v>151</v>
       </c>
-      <c r="E93" s="169"/>
+      <c r="E93" s="168"/>
       <c r="F93" s="108"/>
       <c r="G93" s="55" t="s">
         <v>152</v>
@@ -6681,80 +6847,80 @@
         <v>166</v>
       </c>
       <c r="F94" s="108"/>
-      <c r="G94" s="132"/>
-      <c r="H94" s="133"/>
+      <c r="G94" s="131"/>
+      <c r="H94" s="132"/>
     </row>
     <row r="95" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B95" s="67"/>
-      <c r="C95" s="139"/>
-      <c r="D95" s="140"/>
-      <c r="E95" s="140"/>
-      <c r="F95" s="140"/>
-      <c r="G95" s="140"/>
-      <c r="H95" s="141"/>
+      <c r="C95" s="138"/>
+      <c r="D95" s="139"/>
+      <c r="E95" s="139"/>
+      <c r="F95" s="139"/>
+      <c r="G95" s="139"/>
+      <c r="H95" s="140"/>
     </row>
     <row r="96" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B96" s="67"/>
-      <c r="C96" s="139"/>
-      <c r="D96" s="140"/>
-      <c r="E96" s="140"/>
-      <c r="F96" s="140"/>
-      <c r="G96" s="140"/>
-      <c r="H96" s="141"/>
+      <c r="C96" s="138"/>
+      <c r="D96" s="139"/>
+      <c r="E96" s="139"/>
+      <c r="F96" s="139"/>
+      <c r="G96" s="139"/>
+      <c r="H96" s="140"/>
     </row>
     <row r="97" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="23" t="s">
         <v>39</v>
       </c>
       <c r="B97" s="67"/>
-      <c r="C97" s="139"/>
-      <c r="D97" s="140"/>
-      <c r="E97" s="140"/>
-      <c r="F97" s="140"/>
-      <c r="G97" s="140"/>
-      <c r="H97" s="141"/>
+      <c r="C97" s="138"/>
+      <c r="D97" s="139"/>
+      <c r="E97" s="139"/>
+      <c r="F97" s="139"/>
+      <c r="G97" s="139"/>
+      <c r="H97" s="140"/>
     </row>
     <row r="98" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="23" t="s">
         <v>192</v>
       </c>
       <c r="B98" s="67"/>
-      <c r="C98" s="139"/>
-      <c r="D98" s="140"/>
-      <c r="E98" s="140"/>
-      <c r="F98" s="140"/>
-      <c r="G98" s="140"/>
-      <c r="H98" s="141"/>
+      <c r="C98" s="138"/>
+      <c r="D98" s="139"/>
+      <c r="E98" s="139"/>
+      <c r="F98" s="139"/>
+      <c r="G98" s="139"/>
+      <c r="H98" s="140"/>
     </row>
     <row r="99" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="85" t="s">
         <v>14</v>
       </c>
       <c r="B99" s="86"/>
-      <c r="C99" s="162" t="s">
+      <c r="C99" s="161" t="s">
         <v>155</v>
       </c>
-      <c r="D99" s="163"/>
-      <c r="E99" s="163"/>
-      <c r="F99" s="163"/>
-      <c r="G99" s="163"/>
-      <c r="H99" s="164"/>
+      <c r="D99" s="162"/>
+      <c r="E99" s="162"/>
+      <c r="F99" s="162"/>
+      <c r="G99" s="162"/>
+      <c r="H99" s="163"/>
     </row>
     <row r="100" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B100" s="67"/>
-      <c r="C100" s="139"/>
-      <c r="D100" s="140"/>
-      <c r="E100" s="140"/>
-      <c r="F100" s="159"/>
+      <c r="C100" s="138"/>
+      <c r="D100" s="139"/>
+      <c r="E100" s="139"/>
+      <c r="F100" s="158"/>
       <c r="G100" s="55" t="s">
         <v>173</v>
       </c>
@@ -6765,34 +6931,34 @@
         <v>27</v>
       </c>
       <c r="B101" s="67"/>
-      <c r="C101" s="139"/>
-      <c r="D101" s="140"/>
-      <c r="E101" s="140"/>
-      <c r="F101" s="140"/>
-      <c r="G101" s="140"/>
-      <c r="H101" s="141"/>
+      <c r="C101" s="138"/>
+      <c r="D101" s="139"/>
+      <c r="E101" s="139"/>
+      <c r="F101" s="139"/>
+      <c r="G101" s="139"/>
+      <c r="H101" s="140"/>
     </row>
     <row r="102" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A102" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B102" s="68"/>
-      <c r="C102" s="138"/>
-      <c r="D102" s="135"/>
-      <c r="E102" s="135"/>
-      <c r="F102" s="135"/>
-      <c r="G102" s="135"/>
-      <c r="H102" s="136"/>
+      <c r="C102" s="137"/>
+      <c r="D102" s="134"/>
+      <c r="E102" s="134"/>
+      <c r="F102" s="134"/>
+      <c r="G102" s="134"/>
+      <c r="H102" s="135"/>
     </row>
     <row r="103" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="158"/>
-      <c r="B103" s="158"/>
-      <c r="C103" s="158"/>
-      <c r="D103" s="158"/>
-      <c r="E103" s="158"/>
-      <c r="F103" s="158"/>
-      <c r="G103" s="158"/>
-      <c r="H103" s="158"/>
+      <c r="A103" s="157"/>
+      <c r="B103" s="157"/>
+      <c r="C103" s="157"/>
+      <c r="D103" s="157"/>
+      <c r="E103" s="157"/>
+      <c r="F103" s="157"/>
+      <c r="G103" s="157"/>
+      <c r="H103" s="157"/>
     </row>
     <row r="104" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="25" t="s">
@@ -6801,36 +6967,36 @@
       <c r="B104" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C104" s="145"/>
-      <c r="D104" s="146"/>
-      <c r="E104" s="146"/>
-      <c r="F104" s="146"/>
-      <c r="G104" s="146"/>
-      <c r="H104" s="147"/>
+      <c r="C104" s="144"/>
+      <c r="D104" s="145"/>
+      <c r="E104" s="145"/>
+      <c r="F104" s="145"/>
+      <c r="G104" s="145"/>
+      <c r="H104" s="146"/>
     </row>
     <row r="105" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B105" s="67"/>
-      <c r="C105" s="139"/>
-      <c r="D105" s="140"/>
-      <c r="E105" s="140"/>
-      <c r="F105" s="140"/>
-      <c r="G105" s="140"/>
-      <c r="H105" s="141"/>
+      <c r="C105" s="138"/>
+      <c r="D105" s="139"/>
+      <c r="E105" s="139"/>
+      <c r="F105" s="139"/>
+      <c r="G105" s="139"/>
+      <c r="H105" s="140"/>
     </row>
     <row r="106" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="23" t="s">
         <v>194</v>
       </c>
       <c r="B106" s="67"/>
-      <c r="C106" s="139"/>
-      <c r="D106" s="140"/>
-      <c r="E106" s="140"/>
-      <c r="F106" s="140"/>
-      <c r="G106" s="140"/>
-      <c r="H106" s="141"/>
+      <c r="C106" s="138"/>
+      <c r="D106" s="139"/>
+      <c r="E106" s="139"/>
+      <c r="F106" s="139"/>
+      <c r="G106" s="139"/>
+      <c r="H106" s="140"/>
     </row>
     <row r="107" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="23" t="s">
@@ -6839,12 +7005,12 @@
       <c r="B107" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="C107" s="126"/>
-      <c r="D107" s="142"/>
-      <c r="E107" s="143"/>
-      <c r="F107" s="143"/>
-      <c r="G107" s="143"/>
-      <c r="H107" s="144"/>
+      <c r="C107" s="125"/>
+      <c r="D107" s="141"/>
+      <c r="E107" s="142"/>
+      <c r="F107" s="142"/>
+      <c r="G107" s="142"/>
+      <c r="H107" s="143"/>
     </row>
     <row r="108" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="23" t="s">
@@ -6891,34 +7057,34 @@
         <v>10</v>
       </c>
       <c r="B110" s="67"/>
-      <c r="C110" s="139"/>
-      <c r="D110" s="140"/>
-      <c r="E110" s="140"/>
-      <c r="F110" s="140"/>
-      <c r="G110" s="140"/>
-      <c r="H110" s="141"/>
+      <c r="C110" s="138"/>
+      <c r="D110" s="139"/>
+      <c r="E110" s="139"/>
+      <c r="F110" s="139"/>
+      <c r="G110" s="139"/>
+      <c r="H110" s="140"/>
     </row>
     <row r="111" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A111" s="24" t="s">
         <v>193</v>
       </c>
       <c r="B111" s="68"/>
-      <c r="C111" s="138"/>
-      <c r="D111" s="135"/>
-      <c r="E111" s="135"/>
-      <c r="F111" s="135"/>
-      <c r="G111" s="135"/>
-      <c r="H111" s="136"/>
+      <c r="C111" s="137"/>
+      <c r="D111" s="134"/>
+      <c r="E111" s="134"/>
+      <c r="F111" s="134"/>
+      <c r="G111" s="134"/>
+      <c r="H111" s="135"/>
     </row>
     <row r="112" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="137"/>
-      <c r="B112" s="137"/>
-      <c r="C112" s="137"/>
-      <c r="D112" s="137"/>
-      <c r="E112" s="137"/>
-      <c r="F112" s="137"/>
-      <c r="G112" s="137"/>
-      <c r="H112" s="137"/>
+      <c r="A112" s="136"/>
+      <c r="B112" s="136"/>
+      <c r="C112" s="136"/>
+      <c r="D112" s="136"/>
+      <c r="E112" s="136"/>
+      <c r="F112" s="136"/>
+      <c r="G112" s="136"/>
+      <c r="H112" s="136"/>
     </row>
     <row r="113" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="36" t="s">
@@ -6927,24 +7093,24 @@
       <c r="B113" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C113" s="145"/>
-      <c r="D113" s="146"/>
-      <c r="E113" s="146"/>
-      <c r="F113" s="146"/>
-      <c r="G113" s="146"/>
-      <c r="H113" s="147"/>
+      <c r="C113" s="144"/>
+      <c r="D113" s="145"/>
+      <c r="E113" s="145"/>
+      <c r="F113" s="145"/>
+      <c r="G113" s="145"/>
+      <c r="H113" s="146"/>
     </row>
     <row r="114" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="37" t="s">
         <v>49</v>
       </c>
       <c r="B114" s="46"/>
-      <c r="C114" s="139"/>
-      <c r="D114" s="140"/>
-      <c r="E114" s="140"/>
-      <c r="F114" s="140"/>
-      <c r="G114" s="140"/>
-      <c r="H114" s="141"/>
+      <c r="C114" s="138"/>
+      <c r="D114" s="139"/>
+      <c r="E114" s="139"/>
+      <c r="F114" s="139"/>
+      <c r="G114" s="139"/>
+      <c r="H114" s="140"/>
     </row>
     <row r="115" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="45" t="s">
@@ -6989,22 +7155,22 @@
         <v>50</v>
       </c>
       <c r="B117" s="34"/>
-      <c r="C117" s="138"/>
-      <c r="D117" s="135"/>
-      <c r="E117" s="135"/>
-      <c r="F117" s="135"/>
-      <c r="G117" s="135"/>
-      <c r="H117" s="136"/>
+      <c r="C117" s="137"/>
+      <c r="D117" s="134"/>
+      <c r="E117" s="134"/>
+      <c r="F117" s="134"/>
+      <c r="G117" s="134"/>
+      <c r="H117" s="135"/>
     </row>
     <row r="118" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="137"/>
-      <c r="B118" s="137"/>
-      <c r="C118" s="137"/>
-      <c r="D118" s="137"/>
-      <c r="E118" s="137"/>
-      <c r="F118" s="137"/>
-      <c r="G118" s="137"/>
-      <c r="H118" s="137"/>
+      <c r="A118" s="136"/>
+      <c r="B118" s="136"/>
+      <c r="C118" s="136"/>
+      <c r="D118" s="136"/>
+      <c r="E118" s="136"/>
+      <c r="F118" s="136"/>
+      <c r="G118" s="136"/>
+      <c r="H118" s="136"/>
     </row>
     <row r="119" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="25" t="s">
@@ -7013,50 +7179,50 @@
       <c r="B119" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C119" s="145"/>
-      <c r="D119" s="146"/>
-      <c r="E119" s="146"/>
-      <c r="F119" s="146"/>
-      <c r="G119" s="146"/>
-      <c r="H119" s="147"/>
+      <c r="C119" s="144"/>
+      <c r="D119" s="145"/>
+      <c r="E119" s="145"/>
+      <c r="F119" s="145"/>
+      <c r="G119" s="145"/>
+      <c r="H119" s="146"/>
     </row>
     <row r="120" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="27" t="s">
         <v>65</v>
       </c>
       <c r="B120" s="35"/>
-      <c r="C120" s="139"/>
-      <c r="D120" s="140"/>
-      <c r="E120" s="140"/>
-      <c r="F120" s="140"/>
-      <c r="G120" s="140"/>
-      <c r="H120" s="141"/>
+      <c r="C120" s="138"/>
+      <c r="D120" s="139"/>
+      <c r="E120" s="139"/>
+      <c r="F120" s="139"/>
+      <c r="G120" s="139"/>
+      <c r="H120" s="140"/>
     </row>
     <row r="121" spans="1:8" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A121" s="22" t="s">
         <v>257</v>
       </c>
       <c r="B121" s="35"/>
-      <c r="C121" s="148" t="s">
+      <c r="C121" s="147" t="s">
         <v>259</v>
       </c>
-      <c r="D121" s="149"/>
-      <c r="E121" s="149"/>
-      <c r="F121" s="149"/>
-      <c r="G121" s="149"/>
-      <c r="H121" s="150"/>
+      <c r="D121" s="148"/>
+      <c r="E121" s="148"/>
+      <c r="F121" s="148"/>
+      <c r="G121" s="148"/>
+      <c r="H121" s="149"/>
     </row>
     <row r="122" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A122" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B122" s="33"/>
-      <c r="C122" s="138"/>
-      <c r="D122" s="135"/>
-      <c r="E122" s="135"/>
-      <c r="F122" s="135"/>
-      <c r="G122" s="135"/>
-      <c r="H122" s="136"/>
+      <c r="C122" s="137"/>
+      <c r="D122" s="134"/>
+      <c r="E122" s="134"/>
+      <c r="F122" s="134"/>
+      <c r="G122" s="134"/>
+      <c r="H122" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="130">
@@ -7239,169 +7405,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="123" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="124" t="s">
+      <c r="D1" s="123" t="s">
         <v>227</v>
       </c>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="123" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="123" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="124" t="s">
+      <c r="G1" s="123" t="s">
         <v>229</v>
       </c>
-      <c r="H1" s="124" t="s">
+      <c r="H1" s="123" t="s">
         <v>230</v>
       </c>
-      <c r="I1" s="124" t="s">
+      <c r="I1" s="123" t="s">
         <v>253</v>
       </c>
-      <c r="J1" s="124" t="s">
+      <c r="J1" s="123" t="s">
         <v>208</v>
       </c>
-      <c r="K1" s="124" t="s">
+      <c r="K1" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="124" t="s">
+      <c r="L1" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="M1" s="124" t="s">
+      <c r="M1" s="123" t="s">
         <v>209</v>
       </c>
-      <c r="N1" s="124" t="s">
+      <c r="N1" s="123" t="s">
         <v>233</v>
       </c>
-      <c r="O1" s="124" t="s">
+      <c r="O1" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="P1" s="124" t="s">
+      <c r="P1" s="123" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" s="124" t="s">
+      <c r="Q1" s="123" t="s">
         <v>236</v>
       </c>
-      <c r="R1" s="124" t="s">
+      <c r="R1" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="S1" s="124" t="s">
+      <c r="S1" s="123" t="s">
         <v>238</v>
       </c>
-      <c r="T1" s="124" t="s">
+      <c r="T1" s="123" t="s">
         <v>241</v>
       </c>
-      <c r="U1" s="124" t="s">
+      <c r="U1" s="123" t="s">
         <v>240</v>
       </c>
-      <c r="V1" s="124" t="s">
+      <c r="V1" s="123" t="s">
         <v>239</v>
       </c>
-      <c r="W1" s="124" t="s">
+      <c r="W1" s="123" t="s">
         <v>211</v>
       </c>
-      <c r="X1" s="124" t="s">
+      <c r="X1" s="123" t="s">
         <v>255</v>
       </c>
-      <c r="Y1" s="124" t="s">
+      <c r="Y1" s="123" t="s">
         <v>256</v>
       </c>
-      <c r="Z1" s="124" t="s">
+      <c r="Z1" s="123" t="s">
         <v>212</v>
       </c>
-      <c r="AA1" s="124" t="s">
+      <c r="AA1" s="123" t="s">
         <v>242</v>
       </c>
-      <c r="AB1" s="124" t="s">
+      <c r="AB1" s="123" t="s">
         <v>243</v>
       </c>
-      <c r="AC1" s="124" t="s">
+      <c r="AC1" s="123" t="s">
         <v>213</v>
       </c>
-      <c r="AD1" s="124" t="s">
+      <c r="AD1" s="123" t="s">
         <v>214</v>
       </c>
-      <c r="AE1" s="124" t="s">
+      <c r="AE1" s="123" t="s">
         <v>215</v>
       </c>
-      <c r="AF1" s="124" t="s">
+      <c r="AF1" s="123" t="s">
         <v>216</v>
       </c>
-      <c r="AG1" s="124" t="s">
+      <c r="AG1" s="123" t="s">
         <v>217</v>
       </c>
-      <c r="AH1" s="124" t="s">
+      <c r="AH1" s="123" t="s">
         <v>244</v>
       </c>
-      <c r="AI1" s="124" t="s">
+      <c r="AI1" s="123" t="s">
         <v>245</v>
       </c>
-      <c r="AJ1" s="124" t="s">
+      <c r="AJ1" s="123" t="s">
         <v>246</v>
       </c>
-      <c r="AK1" s="124" t="s">
+      <c r="AK1" s="123" t="s">
         <v>247</v>
       </c>
-      <c r="AL1" s="124" t="s">
+      <c r="AL1" s="123" t="s">
         <v>218</v>
       </c>
-      <c r="AM1" s="124" t="s">
+      <c r="AM1" s="123" t="s">
         <v>219</v>
       </c>
-      <c r="AN1" s="124" t="s">
+      <c r="AN1" s="123" t="s">
         <v>248</v>
       </c>
-      <c r="AO1" s="124" t="s">
+      <c r="AO1" s="123" t="s">
         <v>251</v>
       </c>
-      <c r="AP1" s="124" t="s">
+      <c r="AP1" s="123" t="s">
         <v>250</v>
       </c>
-      <c r="AQ1" s="124" t="s">
+      <c r="AQ1" s="123" t="s">
         <v>249</v>
       </c>
-      <c r="AR1" s="124" t="s">
+      <c r="AR1" s="123" t="s">
         <v>220</v>
       </c>
-      <c r="AS1" s="124" t="s">
+      <c r="AS1" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="AT1" s="124" t="s">
+      <c r="AT1" s="123" t="s">
         <v>222</v>
       </c>
-      <c r="AU1" s="124" t="s">
+      <c r="AU1" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="AV1" s="124" t="s">
+      <c r="AV1" s="123" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="125">
+      <c r="A2" s="124">
         <f>FS_Specs_IC_Powertrain!C3</f>
         <v>0</v>
       </c>
-      <c r="B2" s="125">
+      <c r="B2" s="124">
         <f>FS_Specs_IC_Powertrain!D7</f>
         <v>0</v>
       </c>
-      <c r="C2" s="125">
+      <c r="C2" s="124">
         <f>FS_Specs_IC_Powertrain!F7</f>
         <v>0</v>
       </c>
-      <c r="D2" s="125">
+      <c r="D2" s="124">
         <f>FS_Specs_IC_Powertrain!H7</f>
         <v>0</v>
       </c>
-      <c r="E2" s="125">
+      <c r="E2" s="124">
         <f>FS_Specs_IC_Powertrain!D8</f>
         <v>1550</v>
       </c>
@@ -7409,11 +7575,11 @@
         <f>CONCATENATE(B2,"/",C2,"/",D2,"/",E2)</f>
         <v>0/0/0/1550</v>
       </c>
-      <c r="G2" s="125">
+      <c r="G2" s="124">
         <f>FS_Specs_IC_Powertrain!F8</f>
         <v>1200</v>
       </c>
-      <c r="H2" s="125">
+      <c r="H2" s="124">
         <f>FS_Specs_IC_Powertrain!H8</f>
         <v>1200</v>
       </c>
@@ -7421,15 +7587,15 @@
         <f>CONCATENATE(G2,"/",H2)</f>
         <v>1200/1200</v>
       </c>
-      <c r="J2" s="125">
+      <c r="J2" s="124">
         <f>FS_Specs_IC_Powertrain!H10</f>
         <v>0</v>
       </c>
-      <c r="K2" s="125">
+      <c r="K2" s="124">
         <f>FS_Specs_IC_Powertrain!D10</f>
         <v>0</v>
       </c>
-      <c r="L2" s="125">
+      <c r="L2" s="124">
         <f>FS_Specs_IC_Powertrain!F10</f>
         <v>0</v>
       </c>
@@ -7437,11 +7603,11 @@
         <f>CONCATENATE(K2,"/",L2)</f>
         <v>0/0</v>
       </c>
-      <c r="N2" s="125" t="str">
+      <c r="N2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!C17</f>
         <v xml:space="preserve">Double unequal A-Arm, Coil-over strut suspension, Anti-roll bar		</v>
       </c>
-      <c r="O2" s="125" t="str">
+      <c r="O2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!F17</f>
         <v xml:space="preserve">Double unequal A-Arm, Coil-over strut suspension, Anti-roll bar		</v>
       </c>
@@ -7449,27 +7615,27 @@
         <f>CONCATENATE(N2," ","front","/",O2," ", "rear")</f>
         <v>Double unequal A-Arm, Coil-over strut suspension, Anti-roll bar		 front/Double unequal A-Arm, Coil-over strut suspension, Anti-roll bar		 rear</v>
       </c>
-      <c r="Q2" s="125" t="str">
+      <c r="Q2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!C14</f>
         <v>Avon 7.2/20.0-13</v>
       </c>
-      <c r="R2" s="125">
+      <c r="R2" s="124">
         <f>FS_Specs_IC_Powertrain!D14</f>
         <v>0</v>
       </c>
-      <c r="S2" s="125">
+      <c r="S2" s="124">
         <f>FS_Specs_IC_Powertrain!E14</f>
         <v>0</v>
       </c>
-      <c r="T2" s="125" t="str">
+      <c r="T2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!F14</f>
         <v>Avon 7.2/20.0-13</v>
       </c>
-      <c r="U2" s="125">
+      <c r="U2" s="124">
         <f>FS_Specs_IC_Powertrain!G14</f>
         <v>0</v>
       </c>
-      <c r="V2" s="125">
+      <c r="V2" s="124">
         <f>FS_Specs_IC_Powertrain!H14</f>
         <v>0</v>
       </c>
@@ -7477,11 +7643,11 @@
         <f>CONCATENATE(Q2,"/",R2,"/",S2," ","front","/",T2,"/",U2,"/",V2," ","rear")</f>
         <v>Avon 7.2/20.0-13/0/0 front/Avon 7.2/20.0-13/0/0 rear</v>
       </c>
-      <c r="X2" s="125" t="str">
+      <c r="X2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!C15</f>
         <v>Braid Sturace Monoblock 6" x 13" ET+18</v>
       </c>
-      <c r="Y2" s="125" t="str">
+      <c r="Y2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!F15</f>
         <v>Braid Sturace Monoblock 6" x 13" ET+18</v>
       </c>
@@ -7489,39 +7655,39 @@
         <f>CONCATENATE(X2," ","front","/",Y2," ","rear")</f>
         <v>Braid Sturace Monoblock 6" x 13" ET+18 front/Braid Sturace Monoblock 6" x 13" ET+18 rear</v>
       </c>
-      <c r="AA2" s="125">
+      <c r="AA2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!C41</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="125">
+        <v>16.2mm bore AP Racing CP6465</v>
+      </c>
+      <c r="AB2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!F41</f>
-        <v>0</v>
+        <v>16.2mm bore AP Racing CP6465</v>
       </c>
       <c r="AC2" t="str">
         <f>CONCATENATE(AA2," ","front","/",AB2," ","rear")</f>
-        <v>0 front/0 rear</v>
-      </c>
-      <c r="AD2" s="125">
+        <v>16.2mm bore AP Racing CP6465 front/16.2mm bore AP Racing CP6465 rear</v>
+      </c>
+      <c r="AD2" s="124">
         <f>FS_Specs_IC_Powertrain!C69</f>
         <v>0</v>
       </c>
-      <c r="AE2" s="125">
+      <c r="AE2" s="124">
         <f>FS_Specs_IC_Powertrain!C80</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="125">
+      <c r="AH2" s="124">
         <f>FS_Specs_IC_Powertrain!E83</f>
         <v>0</v>
       </c>
-      <c r="AI2" s="125">
+      <c r="AI2" s="124">
         <f>FS_Specs_IC_Powertrain!H83</f>
         <v>0</v>
       </c>
-      <c r="AJ2" s="125">
+      <c r="AJ2" s="124">
         <f>FS_Specs_IC_Powertrain!E81</f>
         <v>0</v>
       </c>
-      <c r="AK2" s="125">
+      <c r="AK2" s="124">
         <f>FS_Specs_IC_Powertrain!E82</f>
         <v>0</v>
       </c>
@@ -7529,23 +7695,23 @@
         <f>CONCATENATE(AH2,"/",AI2,"/",AJ2,"/",AK2)</f>
         <v>0/0/0/0</v>
       </c>
-      <c r="AM2" s="125">
+      <c r="AM2" s="124">
         <f>FS_Specs_IC_Powertrain!C88</f>
         <v>0</v>
       </c>
-      <c r="AN2" s="125">
+      <c r="AN2" s="124">
         <f>FS_Specs_IC_Powertrain!D84</f>
         <v>0</v>
       </c>
-      <c r="AO2" s="125">
+      <c r="AO2" s="124">
         <f>FS_Specs_IC_Powertrain!D85</f>
         <v>0</v>
       </c>
-      <c r="AP2" s="125">
+      <c r="AP2" s="124">
         <f>FS_Specs_IC_Powertrain!F84</f>
         <v>0</v>
       </c>
-      <c r="AQ2" s="125">
+      <c r="AQ2" s="124">
         <f>FS_Specs_IC_Powertrain!F85</f>
         <v>0</v>
       </c>
@@ -7553,19 +7719,19 @@
         <f>CONCATENATE(AN2,"kW","@",AO2,"rpm","/",AP2,"Nm","@",AQ2,"rpm")</f>
         <v>0kW@0rpm/0Nm@0rpm</v>
       </c>
-      <c r="AS2" s="125">
+      <c r="AS2" s="124">
         <f>FS_Specs_IC_Powertrain!C105</f>
         <v>0</v>
       </c>
-      <c r="AT2" s="125">
+      <c r="AT2" s="124">
         <f>FS_Specs_IC_Powertrain!C106</f>
         <v>0</v>
       </c>
-      <c r="AU2" s="125">
+      <c r="AU2" s="124">
         <f>FS_Specs_IC_Powertrain!C107</f>
         <v>0</v>
       </c>
-      <c r="AV2" s="125" t="str">
+      <c r="AV2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!C121</f>
         <v>E.g. Team xxx from the University of xxx will be aiming for a top 10 finish at this year's Formula Student competition at Silverstone, for their most successful campaign to date.  Established in 2010, the team last enjoyed success in the 2019 competition with their highest placed finish of 11th overall and third best scoring IC team.  Since 2019, focus has been on improved aerodynamics and developing a new braking system.  As well as a top 10 finish, the team will target reaching the Business Plan Presentation finals and finishing Endurance.  Team Leader, xxxxx xxxxxx and the team would like to thank their sponsors xxxx, ssss and rrrrr as well as Faculty Advisor xxxxxxxx and the University of xxx for their continued support of the Formula Student programme.</v>
       </c>

</xml_diff>

<commit_message>
Fully integrated script now outputs all key values, other than those most easily obtained from LLT spreadsheet, which should be fed into the main script.
</commit_message>
<xml_diff>
--- a/2020_fs_design_ic_spec_sheet_-_template.xlsx
+++ b/2020_fs_design_ic_spec_sheet_-_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="FS_Specs_IC_Powertrain" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -116,7 +116,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="10"/>
+            <color rgb="FFFF0000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -125,14 +125,71 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Please do not include other text other than the car number in this field.
-Also, if attending more than one event, please save a separate copy for each competition entry with correct file naming convention and respective car number used on each form.  NOT both numbers in one form.  
-Our systems have difficulty processing text in this field.
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Please do not include other text other than the car number in this field.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Also, if attending more than one event, please save a separate copy for each competition entry with correct file naming convention and respective car number used on each form.  NOT both numbers in one form.  
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Our systems have difficulty processing text in this field.
 </t>
         </r>
       </text>
@@ -1122,13 +1179,61 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Steer Ratio through center.  Be prepared to discuss linearity of ratio (including u-joint effects) with judges. 
-Units:  Hand Wheel Angle:Road Wheel Angle (average left and right)
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steer Ratio through center.  Be prepared to discuss linearity of ratio (including u-joint effects) with judges. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Units:  Hand Wheel Angle:Road Wheel Angle (average left and right)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -2441,7 +2546,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="285">
   <si>
     <t>Car No.</t>
   </si>
@@ -3520,9 +3625,6 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Bracket and shims</t>
   </si>
   <si>
@@ -3553,7 +3655,19 @@
     <t>One-piece rotating hub-axle, machined 6082-T6 w/ 75mm diameter</t>
   </si>
   <si>
-    <t xml:space="preserve">Pair of rubber sealed deep groove 61915-2RS, spaced 3mm		</t>
+    <t xml:space="preserve">Composite Metallic		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sintered Metallic		</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>245 - 255 (248 mm assumed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pair of rubber sealed deep groove 61915-2RS, spaced 5mm		</t>
   </si>
 </sst>
 </file>
@@ -3563,7 +3677,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3720,13 +3834,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="8"/>
       <color indexed="16"/>
       <name val="Franklin Gothic Book"/>
@@ -3776,6 +3883,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -4387,7 +4507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4749,10 +4869,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4760,89 +4880,265 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4853,181 +5149,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -5396,8 +5517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="131" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="131" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5411,15 +5532,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="23" x14ac:dyDescent="0.15">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="162" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
       <c r="H1" s="10">
         <v>2020</v>
       </c>
@@ -5427,56 +5548,56 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="164" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" s="13" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="193"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="184"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" s="13" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="128" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="134"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="213"/>
-      <c r="E4" s="213"/>
-      <c r="F4" s="213"/>
-      <c r="G4" s="213"/>
-      <c r="H4" s="214"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="148"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="136"/>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
+      <c r="A5" s="145"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
     </row>
     <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
@@ -5485,12 +5606,12 @@
       <c r="B6" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
-      <c r="G6" s="179"/>
-      <c r="H6" s="180"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="170"/>
+      <c r="F6" s="170"/>
+      <c r="G6" s="170"/>
+      <c r="H6" s="171"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
@@ -5548,15 +5669,17 @@
       <c r="C9" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="88"/>
+      <c r="D9" s="88" t="s">
+        <v>283</v>
+      </c>
       <c r="E9" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="205" t="s">
+      <c r="F9" s="134" t="s">
         <v>265</v>
       </c>
-      <c r="G9" s="197"/>
-      <c r="H9" s="198"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="132"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
@@ -5568,15 +5691,21 @@
       <c r="C10" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="88"/>
+      <c r="D10" s="88">
+        <v>100</v>
+      </c>
       <c r="E10" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="88"/>
+      <c r="F10" s="88">
+        <v>120</v>
+      </c>
       <c r="G10" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="H10" s="89"/>
+      <c r="H10" s="89">
+        <v>220</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
@@ -5595,17 +5724,17 @@
       <c r="F11" s="90">
         <v>50</v>
       </c>
-      <c r="G11" s="194"/>
-      <c r="H11" s="195"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="186"/>
     </row>
     <row r="12" spans="1:10" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="136"/>
-      <c r="H12" s="136"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
@@ -5614,28 +5743,28 @@
       <c r="B13" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="181" t="s">
+      <c r="C13" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="182"/>
-      <c r="E13" s="183"/>
-      <c r="F13" s="184" t="s">
+      <c r="D13" s="173"/>
+      <c r="E13" s="174"/>
+      <c r="F13" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="182"/>
-      <c r="H13" s="183"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="174"/>
     </row>
     <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
         <v>235</v>
       </c>
       <c r="B14" s="64"/>
-      <c r="C14" s="215" t="s">
+      <c r="C14" s="126" t="s">
         <v>261</v>
       </c>
       <c r="D14" s="84"/>
       <c r="E14" s="87"/>
-      <c r="F14" s="215" t="s">
+      <c r="F14" s="126" t="s">
         <v>261</v>
       </c>
       <c r="G14" s="84"/>
@@ -5648,48 +5777,48 @@
       <c r="B15" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="206" t="s">
+      <c r="C15" s="135" t="s">
         <v>262</v>
       </c>
-      <c r="D15" s="207"/>
-      <c r="E15" s="208"/>
-      <c r="F15" s="206" t="s">
+      <c r="D15" s="136"/>
+      <c r="E15" s="137"/>
+      <c r="F15" s="135" t="s">
         <v>262</v>
       </c>
-      <c r="G15" s="207"/>
-      <c r="H15" s="208"/>
+      <c r="G15" s="136"/>
+      <c r="H15" s="137"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="20" t="s">
         <v>200</v>
       </c>
       <c r="B16" s="64"/>
-      <c r="C16" s="206" t="s">
+      <c r="C16" s="135" t="s">
         <v>263</v>
       </c>
-      <c r="D16" s="207"/>
-      <c r="E16" s="208"/>
-      <c r="F16" s="206" t="s">
+      <c r="D16" s="136"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="135" t="s">
         <v>263</v>
       </c>
-      <c r="G16" s="207"/>
-      <c r="H16" s="208"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="137"/>
     </row>
     <row r="17" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="64"/>
-      <c r="C17" s="203" t="s">
+      <c r="C17" s="130" t="s">
         <v>264</v>
       </c>
-      <c r="D17" s="197"/>
-      <c r="E17" s="198"/>
-      <c r="F17" s="204" t="s">
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="133" t="s">
         <v>264</v>
       </c>
-      <c r="G17" s="197"/>
-      <c r="H17" s="198"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="132"/>
     </row>
     <row r="18" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="20" t="s">
@@ -5724,12 +5853,16 @@
       <c r="B19" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="131"/>
-      <c r="H19" s="132"/>
+      <c r="C19" s="96">
+        <v>13.6</v>
+      </c>
+      <c r="D19" s="140"/>
+      <c r="E19" s="141"/>
+      <c r="F19" s="97">
+        <v>23</v>
+      </c>
+      <c r="G19" s="140"/>
+      <c r="H19" s="141"/>
     </row>
     <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="20" t="s">
@@ -5738,11 +5871,14 @@
       <c r="B20" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="D20" s="131"/>
-      <c r="E20" s="132"/>
+      <c r="C20" s="15">
+        <v>155</v>
+      </c>
+      <c r="D20" s="140"/>
+      <c r="E20" s="141"/>
       <c r="F20" s="97"/>
-      <c r="G20" s="131"/>
-      <c r="H20" s="132"/>
+      <c r="G20" s="140"/>
+      <c r="H20" s="141"/>
     </row>
     <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
@@ -5751,12 +5887,16 @@
       <c r="B21" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="131"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="131"/>
-      <c r="H21" s="132"/>
+      <c r="C21" s="98">
+        <v>2.12</v>
+      </c>
+      <c r="D21" s="140"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="99">
+        <v>2.42</v>
+      </c>
+      <c r="G21" s="140"/>
+      <c r="H21" s="141"/>
     </row>
     <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
@@ -5828,11 +5968,11 @@
       <c r="C25" s="113">
         <v>47.8</v>
       </c>
-      <c r="D25" s="131"/>
-      <c r="E25" s="132"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="141"/>
       <c r="F25" s="38"/>
-      <c r="G25" s="131"/>
-      <c r="H25" s="132"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="141"/>
     </row>
     <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="20" t="s">
@@ -5844,11 +5984,11 @@
       <c r="C26" s="113">
         <v>0.64500000000000002</v>
       </c>
-      <c r="D26" s="131"/>
-      <c r="E26" s="132"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="141"/>
       <c r="F26" s="38"/>
-      <c r="G26" s="131"/>
-      <c r="H26" s="132"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="141"/>
     </row>
     <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="20" t="s">
@@ -5860,13 +6000,13 @@
       <c r="C27" s="100">
         <v>0</v>
       </c>
-      <c r="D27" s="131"/>
-      <c r="E27" s="132"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="141"/>
       <c r="F27" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="G27" s="131"/>
-      <c r="H27" s="132"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="141"/>
     </row>
     <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="20" t="s">
@@ -5878,29 +6018,29 @@
       <c r="C28" s="100">
         <v>-1.5</v>
       </c>
-      <c r="D28" s="131"/>
-      <c r="E28" s="132"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="141"/>
       <c r="F28" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="G28" s="131"/>
-      <c r="H28" s="132"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="141"/>
     </row>
     <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="20" t="s">
         <v>95</v>
       </c>
       <c r="B29" s="64"/>
-      <c r="C29" s="188" t="s">
+      <c r="C29" s="179" t="s">
         <v>267</v>
       </c>
-      <c r="D29" s="139"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="211" t="s">
+      <c r="D29" s="143"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="142" t="s">
         <v>267</v>
       </c>
-      <c r="G29" s="139"/>
-      <c r="H29" s="140"/>
+      <c r="G29" s="143"/>
+      <c r="H29" s="144"/>
     </row>
     <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="20" t="s">
@@ -5912,13 +6052,13 @@
       <c r="C30" s="112">
         <v>0</v>
       </c>
-      <c r="D30" s="131"/>
-      <c r="E30" s="132"/>
+      <c r="D30" s="140"/>
+      <c r="E30" s="141"/>
       <c r="F30" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="G30" s="131"/>
-      <c r="H30" s="132"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="141"/>
     </row>
     <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="20" t="s">
@@ -5930,13 +6070,13 @@
       <c r="C31" s="113">
         <v>29.2</v>
       </c>
-      <c r="D31" s="131"/>
-      <c r="E31" s="132"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="141"/>
       <c r="F31" s="114">
         <v>37.1</v>
       </c>
-      <c r="G31" s="131"/>
-      <c r="H31" s="132"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="141"/>
     </row>
     <row r="32" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
@@ -5948,8 +6088,12 @@
       <c r="C32" s="121" t="s">
         <v>198</v>
       </c>
-      <c r="D32" s="102"/>
-      <c r="E32" s="95"/>
+      <c r="D32" s="102">
+        <v>29.05</v>
+      </c>
+      <c r="E32" s="95">
+        <v>-22.7</v>
+      </c>
       <c r="F32" s="122" t="s">
         <v>199</v>
       </c>
@@ -5997,8 +6141,8 @@
       <c r="F34" s="108">
         <v>53.7</v>
       </c>
-      <c r="G34" s="209"/>
-      <c r="H34" s="210"/>
+      <c r="G34" s="138"/>
+      <c r="H34" s="139"/>
     </row>
     <row r="35" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="20" t="s">
@@ -6014,25 +6158,25 @@
         <v>143</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="F35" s="185"/>
-      <c r="G35" s="186"/>
-      <c r="H35" s="187"/>
+        <v>282</v>
+      </c>
+      <c r="F35" s="176"/>
+      <c r="G35" s="177"/>
+      <c r="H35" s="178"/>
     </row>
     <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="22" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="65"/>
-      <c r="C36" s="196" t="s">
-        <v>271</v>
-      </c>
-      <c r="D36" s="197"/>
-      <c r="E36" s="197"/>
-      <c r="F36" s="197"/>
-      <c r="G36" s="197"/>
-      <c r="H36" s="198"/>
+      <c r="C36" s="161" t="s">
+        <v>270</v>
+      </c>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="132"/>
     </row>
     <row r="37" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
@@ -6048,21 +6192,25 @@
       <c r="E37" s="81" t="s">
         <v>186</v>
       </c>
-      <c r="F37" s="119"/>
+      <c r="F37" s="127">
+        <v>66</v>
+      </c>
       <c r="G37" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="H37" s="120"/>
+      <c r="H37" s="120">
+        <v>70.599999999999994</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="136"/>
-      <c r="B38" s="136"/>
-      <c r="C38" s="136"/>
-      <c r="D38" s="136"/>
-      <c r="E38" s="136"/>
-      <c r="F38" s="136"/>
-      <c r="G38" s="136"/>
-      <c r="H38" s="136"/>
+      <c r="A38" s="145"/>
+      <c r="B38" s="145"/>
+      <c r="C38" s="145"/>
+      <c r="D38" s="145"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="145"/>
     </row>
     <row r="39" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="19" t="s">
@@ -6071,76 +6219,80 @@
       <c r="B39" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="181" t="s">
+      <c r="C39" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="182"/>
-      <c r="E39" s="183"/>
-      <c r="F39" s="181" t="s">
+      <c r="D39" s="173"/>
+      <c r="E39" s="174"/>
+      <c r="F39" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="182"/>
-      <c r="H39" s="183"/>
+      <c r="G39" s="173"/>
+      <c r="H39" s="174"/>
     </row>
     <row r="40" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="40"/>
-      <c r="C40" s="138" t="s">
+      <c r="C40" s="152" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40" s="143"/>
+      <c r="E40" s="144"/>
+      <c r="F40" s="152" t="s">
         <v>272</v>
       </c>
-      <c r="D40" s="139"/>
-      <c r="E40" s="140"/>
-      <c r="F40" s="138" t="s">
-        <v>273</v>
-      </c>
-      <c r="G40" s="139"/>
-      <c r="H40" s="140"/>
+      <c r="G40" s="143"/>
+      <c r="H40" s="144"/>
     </row>
     <row r="41" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="40"/>
-      <c r="C41" s="138" t="s">
-        <v>274</v>
-      </c>
-      <c r="D41" s="139"/>
-      <c r="E41" s="140"/>
-      <c r="F41" s="138" t="s">
-        <v>274</v>
-      </c>
-      <c r="G41" s="139"/>
-      <c r="H41" s="140"/>
+      <c r="C41" s="152" t="s">
+        <v>273</v>
+      </c>
+      <c r="D41" s="143"/>
+      <c r="E41" s="144"/>
+      <c r="F41" s="152" t="s">
+        <v>273</v>
+      </c>
+      <c r="G41" s="143"/>
+      <c r="H41" s="144"/>
     </row>
     <row r="42" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="40"/>
-      <c r="C42" s="138" t="s">
+      <c r="C42" s="152" t="s">
+        <v>274</v>
+      </c>
+      <c r="D42" s="143"/>
+      <c r="E42" s="144"/>
+      <c r="F42" s="152" t="s">
         <v>275</v>
       </c>
-      <c r="D42" s="139"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="138" t="s">
-        <v>276</v>
-      </c>
-      <c r="G42" s="139"/>
-      <c r="H42" s="140"/>
+      <c r="G42" s="143"/>
+      <c r="H42" s="144"/>
     </row>
     <row r="43" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="20" t="s">
         <v>179</v>
       </c>
       <c r="B43" s="40"/>
-      <c r="C43" s="138"/>
-      <c r="D43" s="139"/>
-      <c r="E43" s="140"/>
-      <c r="F43" s="138"/>
-      <c r="G43" s="139"/>
-      <c r="H43" s="140"/>
+      <c r="C43" s="152" t="s">
+        <v>280</v>
+      </c>
+      <c r="D43" s="143"/>
+      <c r="E43" s="144"/>
+      <c r="F43" s="152" t="s">
+        <v>281</v>
+      </c>
+      <c r="G43" s="143"/>
+      <c r="H43" s="144"/>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="20" t="s">
@@ -6150,19 +6302,19 @@
       <c r="C44" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="215">
+      <c r="D44" s="126">
         <v>25.1</v>
       </c>
       <c r="E44" s="56" t="s">
         <v>168</v>
       </c>
-      <c r="F44" s="215">
+      <c r="F44" s="126">
         <v>25.1</v>
       </c>
       <c r="G44" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="H44" s="215">
+      <c r="H44" s="126">
         <v>425</v>
       </c>
     </row>
@@ -6171,58 +6323,58 @@
         <v>36</v>
       </c>
       <c r="B45" s="41"/>
-      <c r="C45" s="138" t="s">
-        <v>277</v>
-      </c>
-      <c r="D45" s="139"/>
-      <c r="E45" s="140"/>
-      <c r="F45" s="138" t="s">
-        <v>277</v>
-      </c>
-      <c r="G45" s="139"/>
-      <c r="H45" s="140"/>
+      <c r="C45" s="152" t="s">
+        <v>276</v>
+      </c>
+      <c r="D45" s="143"/>
+      <c r="E45" s="144"/>
+      <c r="F45" s="152" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45" s="143"/>
+      <c r="H45" s="144"/>
     </row>
     <row r="46" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="40"/>
-      <c r="C46" s="138" t="s">
-        <v>278</v>
-      </c>
-      <c r="D46" s="139"/>
-      <c r="E46" s="140"/>
-      <c r="F46" s="138" t="s">
-        <v>281</v>
-      </c>
-      <c r="G46" s="139"/>
-      <c r="H46" s="140"/>
+      <c r="C46" s="152" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" s="143"/>
+      <c r="E46" s="144"/>
+      <c r="F46" s="152" t="s">
+        <v>284</v>
+      </c>
+      <c r="G46" s="143"/>
+      <c r="H46" s="144"/>
     </row>
     <row r="47" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="42"/>
-      <c r="C47" s="137" t="s">
+      <c r="C47" s="153" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47" s="129"/>
+      <c r="E47" s="154"/>
+      <c r="F47" s="153" t="s">
         <v>279</v>
       </c>
-      <c r="D47" s="134"/>
-      <c r="E47" s="135"/>
-      <c r="F47" s="137" t="s">
-        <v>280</v>
-      </c>
-      <c r="G47" s="134"/>
-      <c r="H47" s="135"/>
+      <c r="G47" s="129"/>
+      <c r="H47" s="154"/>
     </row>
     <row r="48" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="136"/>
-      <c r="B48" s="136"/>
-      <c r="C48" s="136"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="136"/>
-      <c r="F48" s="136"/>
-      <c r="G48" s="136"/>
-      <c r="H48" s="136"/>
+      <c r="A48" s="145"/>
+      <c r="B48" s="145"/>
+      <c r="C48" s="145"/>
+      <c r="D48" s="145"/>
+      <c r="E48" s="145"/>
+      <c r="F48" s="145"/>
+      <c r="G48" s="145"/>
+      <c r="H48" s="145"/>
     </row>
     <row r="49" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="19" t="s">
@@ -6231,36 +6383,36 @@
       <c r="B49" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="144"/>
-      <c r="D49" s="145"/>
-      <c r="E49" s="145"/>
-      <c r="F49" s="145"/>
-      <c r="G49" s="145"/>
-      <c r="H49" s="146"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="156"/>
+      <c r="E49" s="156"/>
+      <c r="F49" s="156"/>
+      <c r="G49" s="156"/>
+      <c r="H49" s="157"/>
     </row>
     <row r="50" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="30"/>
-      <c r="C50" s="127"/>
-      <c r="D50" s="128"/>
-      <c r="E50" s="128"/>
-      <c r="F50" s="128"/>
-      <c r="G50" s="128"/>
-      <c r="H50" s="129"/>
+      <c r="C50" s="149"/>
+      <c r="D50" s="150"/>
+      <c r="E50" s="150"/>
+      <c r="F50" s="150"/>
+      <c r="G50" s="150"/>
+      <c r="H50" s="151"/>
     </row>
     <row r="51" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="30"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="128"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="128"/>
-      <c r="G51" s="128"/>
-      <c r="H51" s="129"/>
+      <c r="C51" s="149"/>
+      <c r="D51" s="150"/>
+      <c r="E51" s="150"/>
+      <c r="F51" s="150"/>
+      <c r="G51" s="150"/>
+      <c r="H51" s="151"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="20" t="s">
@@ -6274,77 +6426,77 @@
       <c r="E52" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="F52" s="199"/>
-      <c r="G52" s="200"/>
-      <c r="H52" s="201"/>
+      <c r="F52" s="158"/>
+      <c r="G52" s="159"/>
+      <c r="H52" s="160"/>
     </row>
     <row r="53" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="30"/>
-      <c r="C53" s="127"/>
-      <c r="D53" s="128"/>
-      <c r="E53" s="128"/>
-      <c r="F53" s="128"/>
-      <c r="G53" s="128"/>
-      <c r="H53" s="129"/>
+      <c r="C53" s="149"/>
+      <c r="D53" s="150"/>
+      <c r="E53" s="150"/>
+      <c r="F53" s="150"/>
+      <c r="G53" s="150"/>
+      <c r="H53" s="151"/>
     </row>
     <row r="54" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B54" s="30"/>
-      <c r="C54" s="127"/>
-      <c r="D54" s="128"/>
-      <c r="E54" s="128"/>
-      <c r="F54" s="128"/>
-      <c r="G54" s="128"/>
-      <c r="H54" s="129"/>
+      <c r="C54" s="149"/>
+      <c r="D54" s="150"/>
+      <c r="E54" s="150"/>
+      <c r="F54" s="150"/>
+      <c r="G54" s="150"/>
+      <c r="H54" s="151"/>
     </row>
     <row r="55" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B55" s="30"/>
-      <c r="C55" s="127"/>
-      <c r="D55" s="128"/>
-      <c r="E55" s="128"/>
-      <c r="F55" s="128"/>
-      <c r="G55" s="128"/>
-      <c r="H55" s="129"/>
+      <c r="C55" s="149"/>
+      <c r="D55" s="150"/>
+      <c r="E55" s="150"/>
+      <c r="F55" s="150"/>
+      <c r="G55" s="150"/>
+      <c r="H55" s="151"/>
     </row>
     <row r="56" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="79" t="s">
         <v>178</v>
       </c>
       <c r="B56" s="80"/>
-      <c r="C56" s="175"/>
-      <c r="D56" s="176"/>
-      <c r="E56" s="176"/>
-      <c r="F56" s="176"/>
-      <c r="G56" s="176"/>
-      <c r="H56" s="177"/>
+      <c r="C56" s="166"/>
+      <c r="D56" s="167"/>
+      <c r="E56" s="167"/>
+      <c r="F56" s="167"/>
+      <c r="G56" s="167"/>
+      <c r="H56" s="168"/>
     </row>
     <row r="57" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="130"/>
-      <c r="B57" s="130"/>
-      <c r="C57" s="130"/>
-      <c r="D57" s="130"/>
-      <c r="E57" s="130"/>
-      <c r="F57" s="130"/>
-      <c r="G57" s="130"/>
-      <c r="H57" s="130"/>
+      <c r="A57" s="206"/>
+      <c r="B57" s="206"/>
+      <c r="C57" s="206"/>
+      <c r="D57" s="206"/>
+      <c r="E57" s="206"/>
+      <c r="F57" s="206"/>
+      <c r="G57" s="206"/>
+      <c r="H57" s="206"/>
     </row>
     <row r="58" spans="1:8" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="126"/>
-      <c r="B58" s="126"/>
-      <c r="C58" s="126"/>
-      <c r="D58" s="126"/>
-      <c r="E58" s="126"/>
-      <c r="F58" s="126"/>
-      <c r="G58" s="126"/>
-      <c r="H58" s="126"/>
+      <c r="A58" s="205"/>
+      <c r="B58" s="205"/>
+      <c r="C58" s="205"/>
+      <c r="D58" s="205"/>
+      <c r="E58" s="205"/>
+      <c r="F58" s="205"/>
+      <c r="G58" s="205"/>
+      <c r="H58" s="205"/>
     </row>
     <row r="59" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="19" t="s">
@@ -6353,106 +6505,106 @@
       <c r="B59" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="144"/>
-      <c r="D59" s="145"/>
-      <c r="E59" s="145"/>
-      <c r="F59" s="145"/>
-      <c r="G59" s="145"/>
-      <c r="H59" s="146"/>
+      <c r="C59" s="155"/>
+      <c r="D59" s="156"/>
+      <c r="E59" s="156"/>
+      <c r="F59" s="156"/>
+      <c r="G59" s="156"/>
+      <c r="H59" s="157"/>
     </row>
     <row r="60" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="20" t="s">
         <v>175</v>
       </c>
       <c r="B60" s="31"/>
-      <c r="C60" s="127"/>
-      <c r="D60" s="128"/>
-      <c r="E60" s="128"/>
-      <c r="F60" s="128"/>
-      <c r="G60" s="128"/>
-      <c r="H60" s="129"/>
+      <c r="C60" s="149"/>
+      <c r="D60" s="150"/>
+      <c r="E60" s="150"/>
+      <c r="F60" s="150"/>
+      <c r="G60" s="150"/>
+      <c r="H60" s="151"/>
     </row>
     <row r="61" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="31"/>
-      <c r="C61" s="127"/>
-      <c r="D61" s="128"/>
-      <c r="E61" s="128"/>
-      <c r="F61" s="128"/>
-      <c r="G61" s="128"/>
-      <c r="H61" s="129"/>
+      <c r="C61" s="149"/>
+      <c r="D61" s="150"/>
+      <c r="E61" s="150"/>
+      <c r="F61" s="150"/>
+      <c r="G61" s="150"/>
+      <c r="H61" s="151"/>
     </row>
     <row r="62" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="20" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="31"/>
-      <c r="C62" s="127"/>
-      <c r="D62" s="128"/>
-      <c r="E62" s="128"/>
-      <c r="F62" s="128"/>
-      <c r="G62" s="128"/>
-      <c r="H62" s="129"/>
+      <c r="C62" s="149"/>
+      <c r="D62" s="150"/>
+      <c r="E62" s="150"/>
+      <c r="F62" s="150"/>
+      <c r="G62" s="150"/>
+      <c r="H62" s="151"/>
     </row>
     <row r="63" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B63" s="30"/>
-      <c r="C63" s="127"/>
-      <c r="D63" s="128"/>
-      <c r="E63" s="128"/>
-      <c r="F63" s="128"/>
-      <c r="G63" s="128"/>
-      <c r="H63" s="129"/>
+      <c r="C63" s="149"/>
+      <c r="D63" s="150"/>
+      <c r="E63" s="150"/>
+      <c r="F63" s="150"/>
+      <c r="G63" s="150"/>
+      <c r="H63" s="151"/>
     </row>
     <row r="64" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="20" t="s">
         <v>51</v>
       </c>
       <c r="B64" s="31"/>
-      <c r="C64" s="127"/>
-      <c r="D64" s="128"/>
-      <c r="E64" s="128"/>
-      <c r="F64" s="128"/>
-      <c r="G64" s="128"/>
-      <c r="H64" s="129"/>
+      <c r="C64" s="149"/>
+      <c r="D64" s="150"/>
+      <c r="E64" s="150"/>
+      <c r="F64" s="150"/>
+      <c r="G64" s="150"/>
+      <c r="H64" s="151"/>
     </row>
     <row r="65" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="20" t="s">
         <v>55</v>
       </c>
       <c r="B65" s="31"/>
-      <c r="C65" s="127"/>
-      <c r="D65" s="128"/>
-      <c r="E65" s="128"/>
-      <c r="F65" s="128"/>
-      <c r="G65" s="128"/>
-      <c r="H65" s="129"/>
+      <c r="C65" s="149"/>
+      <c r="D65" s="150"/>
+      <c r="E65" s="150"/>
+      <c r="F65" s="150"/>
+      <c r="G65" s="150"/>
+      <c r="H65" s="151"/>
     </row>
     <row r="66" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B66" s="32"/>
-      <c r="C66" s="154"/>
-      <c r="D66" s="155"/>
-      <c r="E66" s="155"/>
-      <c r="F66" s="155"/>
-      <c r="G66" s="155"/>
-      <c r="H66" s="156"/>
+      <c r="C66" s="214"/>
+      <c r="D66" s="215"/>
+      <c r="E66" s="215"/>
+      <c r="F66" s="215"/>
+      <c r="G66" s="215"/>
+      <c r="H66" s="216"/>
     </row>
     <row r="67" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="136"/>
-      <c r="B67" s="136"/>
-      <c r="C67" s="136"/>
-      <c r="D67" s="136"/>
-      <c r="E67" s="136"/>
-      <c r="F67" s="136"/>
-      <c r="G67" s="136"/>
-      <c r="H67" s="136"/>
+      <c r="A67" s="145"/>
+      <c r="B67" s="145"/>
+      <c r="C67" s="145"/>
+      <c r="D67" s="145"/>
+      <c r="E67" s="145"/>
+      <c r="F67" s="145"/>
+      <c r="G67" s="145"/>
+      <c r="H67" s="145"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="19" t="s">
@@ -6461,48 +6613,48 @@
       <c r="B68" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C68" s="144"/>
-      <c r="D68" s="145"/>
-      <c r="E68" s="145"/>
-      <c r="F68" s="145"/>
-      <c r="G68" s="145"/>
-      <c r="H68" s="146"/>
+      <c r="C68" s="155"/>
+      <c r="D68" s="156"/>
+      <c r="E68" s="156"/>
+      <c r="F68" s="156"/>
+      <c r="G68" s="156"/>
+      <c r="H68" s="157"/>
     </row>
     <row r="69" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B69" s="67"/>
-      <c r="C69" s="127"/>
-      <c r="D69" s="128"/>
-      <c r="E69" s="128"/>
-      <c r="F69" s="128"/>
-      <c r="G69" s="128"/>
-      <c r="H69" s="129"/>
+      <c r="C69" s="149"/>
+      <c r="D69" s="150"/>
+      <c r="E69" s="150"/>
+      <c r="F69" s="150"/>
+      <c r="G69" s="150"/>
+      <c r="H69" s="151"/>
     </row>
     <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B70" s="67"/>
-      <c r="C70" s="127"/>
-      <c r="D70" s="128"/>
-      <c r="E70" s="128"/>
-      <c r="F70" s="128"/>
-      <c r="G70" s="128"/>
-      <c r="H70" s="129"/>
+      <c r="C70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="150"/>
+      <c r="F70" s="150"/>
+      <c r="G70" s="150"/>
+      <c r="H70" s="151"/>
     </row>
     <row r="71" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B71" s="67"/>
-      <c r="C71" s="127"/>
-      <c r="D71" s="128"/>
-      <c r="E71" s="128"/>
-      <c r="F71" s="128"/>
-      <c r="G71" s="128"/>
-      <c r="H71" s="129"/>
+      <c r="C71" s="149"/>
+      <c r="D71" s="150"/>
+      <c r="E71" s="150"/>
+      <c r="F71" s="150"/>
+      <c r="G71" s="150"/>
+      <c r="H71" s="151"/>
     </row>
     <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="23" t="s">
@@ -6519,8 +6671,8 @@
         <v>108</v>
       </c>
       <c r="F72" s="108"/>
-      <c r="G72" s="131"/>
-      <c r="H72" s="132"/>
+      <c r="G72" s="140"/>
+      <c r="H72" s="141"/>
     </row>
     <row r="73" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="23" t="s">
@@ -6547,24 +6699,24 @@
         <v>104</v>
       </c>
       <c r="B74" s="67"/>
-      <c r="C74" s="127"/>
-      <c r="D74" s="128"/>
-      <c r="E74" s="128"/>
-      <c r="F74" s="128"/>
-      <c r="G74" s="128"/>
-      <c r="H74" s="129"/>
+      <c r="C74" s="149"/>
+      <c r="D74" s="150"/>
+      <c r="E74" s="150"/>
+      <c r="F74" s="150"/>
+      <c r="G74" s="150"/>
+      <c r="H74" s="151"/>
     </row>
     <row r="75" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="23" t="s">
         <v>167</v>
       </c>
       <c r="B75" s="67"/>
-      <c r="C75" s="127"/>
-      <c r="D75" s="128"/>
-      <c r="E75" s="128"/>
-      <c r="F75" s="128"/>
-      <c r="G75" s="128"/>
-      <c r="H75" s="129"/>
+      <c r="C75" s="149"/>
+      <c r="D75" s="150"/>
+      <c r="E75" s="150"/>
+      <c r="F75" s="150"/>
+      <c r="G75" s="150"/>
+      <c r="H75" s="151"/>
     </row>
     <row r="76" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="23" t="s">
@@ -6600,19 +6752,19 @@
       <c r="E77" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" s="133"/>
-      <c r="G77" s="134"/>
-      <c r="H77" s="135"/>
+      <c r="F77" s="207"/>
+      <c r="G77" s="129"/>
+      <c r="H77" s="154"/>
     </row>
     <row r="78" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="157"/>
-      <c r="B78" s="157"/>
-      <c r="C78" s="157"/>
-      <c r="D78" s="157"/>
-      <c r="E78" s="157"/>
-      <c r="F78" s="157"/>
-      <c r="G78" s="157"/>
-      <c r="H78" s="157"/>
+      <c r="A78" s="189"/>
+      <c r="B78" s="189"/>
+      <c r="C78" s="189"/>
+      <c r="D78" s="189"/>
+      <c r="E78" s="189"/>
+      <c r="F78" s="189"/>
+      <c r="G78" s="189"/>
+      <c r="H78" s="189"/>
     </row>
     <row r="79" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="25" t="s">
@@ -6621,39 +6773,39 @@
       <c r="B79" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="144"/>
-      <c r="D79" s="145"/>
-      <c r="E79" s="145"/>
-      <c r="F79" s="145"/>
-      <c r="G79" s="145"/>
-      <c r="H79" s="146"/>
+      <c r="C79" s="155"/>
+      <c r="D79" s="156"/>
+      <c r="E79" s="156"/>
+      <c r="F79" s="156"/>
+      <c r="G79" s="156"/>
+      <c r="H79" s="157"/>
     </row>
     <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B80" s="67"/>
-      <c r="C80" s="138"/>
-      <c r="D80" s="139"/>
-      <c r="E80" s="139"/>
-      <c r="F80" s="139"/>
-      <c r="G80" s="139"/>
-      <c r="H80" s="140"/>
+      <c r="C80" s="152"/>
+      <c r="D80" s="143"/>
+      <c r="E80" s="143"/>
+      <c r="F80" s="143"/>
+      <c r="G80" s="143"/>
+      <c r="H80" s="144"/>
     </row>
     <row r="81" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="23" t="s">
         <v>116</v>
       </c>
       <c r="B81" s="67"/>
-      <c r="C81" s="150" t="s">
+      <c r="C81" s="203" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="151"/>
+      <c r="D81" s="204"/>
       <c r="E81" s="91"/>
-      <c r="F81" s="152" t="s">
+      <c r="F81" s="187" t="s">
         <v>172</v>
       </c>
-      <c r="G81" s="153"/>
+      <c r="G81" s="188"/>
       <c r="H81" s="48"/>
     </row>
     <row r="82" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -6661,15 +6813,15 @@
         <v>115</v>
       </c>
       <c r="B82" s="67"/>
-      <c r="C82" s="150" t="s">
+      <c r="C82" s="203" t="s">
         <v>112</v>
       </c>
-      <c r="D82" s="151"/>
+      <c r="D82" s="204"/>
       <c r="E82" s="91"/>
-      <c r="F82" s="152" t="s">
+      <c r="F82" s="187" t="s">
         <v>113</v>
       </c>
-      <c r="G82" s="153"/>
+      <c r="G82" s="188"/>
       <c r="H82" s="95"/>
     </row>
     <row r="83" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -6679,15 +6831,15 @@
       <c r="B83" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="150" t="s">
+      <c r="C83" s="203" t="s">
         <v>153</v>
       </c>
-      <c r="D83" s="151"/>
+      <c r="D83" s="204"/>
       <c r="E83" s="102"/>
-      <c r="F83" s="152">
+      <c r="F83" s="187">
         <v>84.5</v>
       </c>
-      <c r="G83" s="153"/>
+      <c r="G83" s="188"/>
       <c r="H83" s="95"/>
     </row>
     <row r="84" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -6703,8 +6855,8 @@
         <v>164</v>
       </c>
       <c r="F84" s="17"/>
-      <c r="G84" s="169"/>
-      <c r="H84" s="170"/>
+      <c r="G84" s="201"/>
+      <c r="H84" s="202"/>
     </row>
     <row r="85" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="23" t="s">
@@ -6731,48 +6883,48 @@
         <v>48</v>
       </c>
       <c r="B86" s="67"/>
-      <c r="C86" s="138"/>
-      <c r="D86" s="139"/>
-      <c r="E86" s="139"/>
-      <c r="F86" s="139"/>
-      <c r="G86" s="139"/>
-      <c r="H86" s="140"/>
+      <c r="C86" s="152"/>
+      <c r="D86" s="143"/>
+      <c r="E86" s="143"/>
+      <c r="F86" s="143"/>
+      <c r="G86" s="143"/>
+      <c r="H86" s="144"/>
     </row>
     <row r="87" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="23" t="s">
         <v>46</v>
       </c>
       <c r="B87" s="67"/>
-      <c r="C87" s="138"/>
-      <c r="D87" s="139"/>
-      <c r="E87" s="139"/>
-      <c r="F87" s="139"/>
-      <c r="G87" s="139"/>
-      <c r="H87" s="140"/>
+      <c r="C87" s="152"/>
+      <c r="D87" s="143"/>
+      <c r="E87" s="143"/>
+      <c r="F87" s="143"/>
+      <c r="G87" s="143"/>
+      <c r="H87" s="144"/>
     </row>
     <row r="88" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B88" s="67"/>
-      <c r="C88" s="138"/>
-      <c r="D88" s="139"/>
-      <c r="E88" s="139"/>
-      <c r="F88" s="139"/>
-      <c r="G88" s="139"/>
-      <c r="H88" s="140"/>
+      <c r="C88" s="152"/>
+      <c r="D88" s="143"/>
+      <c r="E88" s="143"/>
+      <c r="F88" s="143"/>
+      <c r="G88" s="143"/>
+      <c r="H88" s="144"/>
     </row>
     <row r="89" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="23" t="s">
         <v>123</v>
       </c>
       <c r="B89" s="67"/>
-      <c r="C89" s="138"/>
-      <c r="D89" s="139"/>
-      <c r="E89" s="139"/>
-      <c r="F89" s="139"/>
-      <c r="G89" s="139"/>
-      <c r="H89" s="140"/>
+      <c r="C89" s="152"/>
+      <c r="D89" s="143"/>
+      <c r="E89" s="143"/>
+      <c r="F89" s="143"/>
+      <c r="G89" s="143"/>
+      <c r="H89" s="144"/>
     </row>
     <row r="90" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="23" t="s">
@@ -6782,25 +6934,25 @@
         <v>80</v>
       </c>
       <c r="C90" s="44"/>
-      <c r="D90" s="164"/>
-      <c r="E90" s="165"/>
-      <c r="F90" s="165"/>
-      <c r="G90" s="165"/>
-      <c r="H90" s="166"/>
+      <c r="D90" s="196"/>
+      <c r="E90" s="197"/>
+      <c r="F90" s="197"/>
+      <c r="G90" s="197"/>
+      <c r="H90" s="198"/>
     </row>
     <row r="91" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B91" s="67"/>
-      <c r="C91" s="138" t="s">
+      <c r="C91" s="152" t="s">
         <v>62</v>
       </c>
-      <c r="D91" s="139"/>
-      <c r="E91" s="139"/>
-      <c r="F91" s="139"/>
-      <c r="G91" s="139"/>
-      <c r="H91" s="140"/>
+      <c r="D91" s="143"/>
+      <c r="E91" s="143"/>
+      <c r="F91" s="143"/>
+      <c r="G91" s="143"/>
+      <c r="H91" s="144"/>
     </row>
     <row r="92" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="23" t="s">
@@ -6811,10 +6963,10 @@
         <v>121</v>
       </c>
       <c r="D92" s="109"/>
-      <c r="E92" s="159" t="s">
+      <c r="E92" s="191" t="s">
         <v>120</v>
       </c>
-      <c r="F92" s="160"/>
+      <c r="F92" s="192"/>
       <c r="G92" s="94"/>
       <c r="H92" s="50"/>
     </row>
@@ -6824,10 +6976,10 @@
       </c>
       <c r="B93" s="67"/>
       <c r="C93" s="44"/>
-      <c r="D93" s="167" t="s">
+      <c r="D93" s="199" t="s">
         <v>151</v>
       </c>
-      <c r="E93" s="168"/>
+      <c r="E93" s="200"/>
       <c r="F93" s="108"/>
       <c r="G93" s="55" t="s">
         <v>152</v>
@@ -6847,80 +6999,80 @@
         <v>166</v>
       </c>
       <c r="F94" s="108"/>
-      <c r="G94" s="131"/>
-      <c r="H94" s="132"/>
+      <c r="G94" s="140"/>
+      <c r="H94" s="141"/>
     </row>
     <row r="95" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B95" s="67"/>
-      <c r="C95" s="138"/>
-      <c r="D95" s="139"/>
-      <c r="E95" s="139"/>
-      <c r="F95" s="139"/>
-      <c r="G95" s="139"/>
-      <c r="H95" s="140"/>
+      <c r="C95" s="152"/>
+      <c r="D95" s="143"/>
+      <c r="E95" s="143"/>
+      <c r="F95" s="143"/>
+      <c r="G95" s="143"/>
+      <c r="H95" s="144"/>
     </row>
     <row r="96" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B96" s="67"/>
-      <c r="C96" s="138"/>
-      <c r="D96" s="139"/>
-      <c r="E96" s="139"/>
-      <c r="F96" s="139"/>
-      <c r="G96" s="139"/>
-      <c r="H96" s="140"/>
+      <c r="C96" s="152"/>
+      <c r="D96" s="143"/>
+      <c r="E96" s="143"/>
+      <c r="F96" s="143"/>
+      <c r="G96" s="143"/>
+      <c r="H96" s="144"/>
     </row>
     <row r="97" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="23" t="s">
         <v>39</v>
       </c>
       <c r="B97" s="67"/>
-      <c r="C97" s="138"/>
-      <c r="D97" s="139"/>
-      <c r="E97" s="139"/>
-      <c r="F97" s="139"/>
-      <c r="G97" s="139"/>
-      <c r="H97" s="140"/>
+      <c r="C97" s="152"/>
+      <c r="D97" s="143"/>
+      <c r="E97" s="143"/>
+      <c r="F97" s="143"/>
+      <c r="G97" s="143"/>
+      <c r="H97" s="144"/>
     </row>
     <row r="98" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="23" t="s">
         <v>192</v>
       </c>
       <c r="B98" s="67"/>
-      <c r="C98" s="138"/>
-      <c r="D98" s="139"/>
-      <c r="E98" s="139"/>
-      <c r="F98" s="139"/>
-      <c r="G98" s="139"/>
-      <c r="H98" s="140"/>
+      <c r="C98" s="152"/>
+      <c r="D98" s="143"/>
+      <c r="E98" s="143"/>
+      <c r="F98" s="143"/>
+      <c r="G98" s="143"/>
+      <c r="H98" s="144"/>
     </row>
     <row r="99" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="85" t="s">
         <v>14</v>
       </c>
       <c r="B99" s="86"/>
-      <c r="C99" s="161" t="s">
+      <c r="C99" s="193" t="s">
         <v>155</v>
       </c>
-      <c r="D99" s="162"/>
-      <c r="E99" s="162"/>
-      <c r="F99" s="162"/>
-      <c r="G99" s="162"/>
-      <c r="H99" s="163"/>
+      <c r="D99" s="194"/>
+      <c r="E99" s="194"/>
+      <c r="F99" s="194"/>
+      <c r="G99" s="194"/>
+      <c r="H99" s="195"/>
     </row>
     <row r="100" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B100" s="67"/>
-      <c r="C100" s="138"/>
-      <c r="D100" s="139"/>
-      <c r="E100" s="139"/>
-      <c r="F100" s="158"/>
+      <c r="C100" s="152"/>
+      <c r="D100" s="143"/>
+      <c r="E100" s="143"/>
+      <c r="F100" s="190"/>
       <c r="G100" s="55" t="s">
         <v>173</v>
       </c>
@@ -6931,34 +7083,34 @@
         <v>27</v>
       </c>
       <c r="B101" s="67"/>
-      <c r="C101" s="138"/>
-      <c r="D101" s="139"/>
-      <c r="E101" s="139"/>
-      <c r="F101" s="139"/>
-      <c r="G101" s="139"/>
-      <c r="H101" s="140"/>
+      <c r="C101" s="152"/>
+      <c r="D101" s="143"/>
+      <c r="E101" s="143"/>
+      <c r="F101" s="143"/>
+      <c r="G101" s="143"/>
+      <c r="H101" s="144"/>
     </row>
     <row r="102" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A102" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B102" s="68"/>
-      <c r="C102" s="137"/>
-      <c r="D102" s="134"/>
-      <c r="E102" s="134"/>
-      <c r="F102" s="134"/>
-      <c r="G102" s="134"/>
-      <c r="H102" s="135"/>
+      <c r="C102" s="153"/>
+      <c r="D102" s="129"/>
+      <c r="E102" s="129"/>
+      <c r="F102" s="129"/>
+      <c r="G102" s="129"/>
+      <c r="H102" s="154"/>
     </row>
     <row r="103" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="157"/>
-      <c r="B103" s="157"/>
-      <c r="C103" s="157"/>
-      <c r="D103" s="157"/>
-      <c r="E103" s="157"/>
-      <c r="F103" s="157"/>
-      <c r="G103" s="157"/>
-      <c r="H103" s="157"/>
+      <c r="A103" s="189"/>
+      <c r="B103" s="189"/>
+      <c r="C103" s="189"/>
+      <c r="D103" s="189"/>
+      <c r="E103" s="189"/>
+      <c r="F103" s="189"/>
+      <c r="G103" s="189"/>
+      <c r="H103" s="189"/>
     </row>
     <row r="104" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="25" t="s">
@@ -6967,36 +7119,36 @@
       <c r="B104" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C104" s="144"/>
-      <c r="D104" s="145"/>
-      <c r="E104" s="145"/>
-      <c r="F104" s="145"/>
-      <c r="G104" s="145"/>
-      <c r="H104" s="146"/>
+      <c r="C104" s="155"/>
+      <c r="D104" s="156"/>
+      <c r="E104" s="156"/>
+      <c r="F104" s="156"/>
+      <c r="G104" s="156"/>
+      <c r="H104" s="157"/>
     </row>
     <row r="105" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B105" s="67"/>
-      <c r="C105" s="138"/>
-      <c r="D105" s="139"/>
-      <c r="E105" s="139"/>
-      <c r="F105" s="139"/>
-      <c r="G105" s="139"/>
-      <c r="H105" s="140"/>
+      <c r="C105" s="152"/>
+      <c r="D105" s="143"/>
+      <c r="E105" s="143"/>
+      <c r="F105" s="143"/>
+      <c r="G105" s="143"/>
+      <c r="H105" s="144"/>
     </row>
     <row r="106" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="23" t="s">
         <v>194</v>
       </c>
       <c r="B106" s="67"/>
-      <c r="C106" s="138"/>
-      <c r="D106" s="139"/>
-      <c r="E106" s="139"/>
-      <c r="F106" s="139"/>
-      <c r="G106" s="139"/>
-      <c r="H106" s="140"/>
+      <c r="C106" s="152"/>
+      <c r="D106" s="143"/>
+      <c r="E106" s="143"/>
+      <c r="F106" s="143"/>
+      <c r="G106" s="143"/>
+      <c r="H106" s="144"/>
     </row>
     <row r="107" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="23" t="s">
@@ -7006,11 +7158,11 @@
         <v>100</v>
       </c>
       <c r="C107" s="125"/>
-      <c r="D107" s="141"/>
-      <c r="E107" s="142"/>
-      <c r="F107" s="142"/>
-      <c r="G107" s="142"/>
-      <c r="H107" s="143"/>
+      <c r="D107" s="208"/>
+      <c r="E107" s="209"/>
+      <c r="F107" s="209"/>
+      <c r="G107" s="209"/>
+      <c r="H107" s="210"/>
     </row>
     <row r="108" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="23" t="s">
@@ -7057,34 +7209,34 @@
         <v>10</v>
       </c>
       <c r="B110" s="67"/>
-      <c r="C110" s="138"/>
-      <c r="D110" s="139"/>
-      <c r="E110" s="139"/>
-      <c r="F110" s="139"/>
-      <c r="G110" s="139"/>
-      <c r="H110" s="140"/>
+      <c r="C110" s="152"/>
+      <c r="D110" s="143"/>
+      <c r="E110" s="143"/>
+      <c r="F110" s="143"/>
+      <c r="G110" s="143"/>
+      <c r="H110" s="144"/>
     </row>
     <row r="111" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A111" s="24" t="s">
         <v>193</v>
       </c>
       <c r="B111" s="68"/>
-      <c r="C111" s="137"/>
-      <c r="D111" s="134"/>
-      <c r="E111" s="134"/>
-      <c r="F111" s="134"/>
-      <c r="G111" s="134"/>
-      <c r="H111" s="135"/>
+      <c r="C111" s="153"/>
+      <c r="D111" s="129"/>
+      <c r="E111" s="129"/>
+      <c r="F111" s="129"/>
+      <c r="G111" s="129"/>
+      <c r="H111" s="154"/>
     </row>
     <row r="112" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="136"/>
-      <c r="B112" s="136"/>
-      <c r="C112" s="136"/>
-      <c r="D112" s="136"/>
-      <c r="E112" s="136"/>
-      <c r="F112" s="136"/>
-      <c r="G112" s="136"/>
-      <c r="H112" s="136"/>
+      <c r="A112" s="145"/>
+      <c r="B112" s="145"/>
+      <c r="C112" s="145"/>
+      <c r="D112" s="145"/>
+      <c r="E112" s="145"/>
+      <c r="F112" s="145"/>
+      <c r="G112" s="145"/>
+      <c r="H112" s="145"/>
     </row>
     <row r="113" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="36" t="s">
@@ -7093,24 +7245,24 @@
       <c r="B113" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C113" s="144"/>
-      <c r="D113" s="145"/>
-      <c r="E113" s="145"/>
-      <c r="F113" s="145"/>
-      <c r="G113" s="145"/>
-      <c r="H113" s="146"/>
+      <c r="C113" s="155"/>
+      <c r="D113" s="156"/>
+      <c r="E113" s="156"/>
+      <c r="F113" s="156"/>
+      <c r="G113" s="156"/>
+      <c r="H113" s="157"/>
     </row>
     <row r="114" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="37" t="s">
         <v>49</v>
       </c>
       <c r="B114" s="46"/>
-      <c r="C114" s="138"/>
-      <c r="D114" s="139"/>
-      <c r="E114" s="139"/>
-      <c r="F114" s="139"/>
-      <c r="G114" s="139"/>
-      <c r="H114" s="140"/>
+      <c r="C114" s="152"/>
+      <c r="D114" s="143"/>
+      <c r="E114" s="143"/>
+      <c r="F114" s="143"/>
+      <c r="G114" s="143"/>
+      <c r="H114" s="144"/>
     </row>
     <row r="115" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="45" t="s">
@@ -7155,22 +7307,22 @@
         <v>50</v>
       </c>
       <c r="B117" s="34"/>
-      <c r="C117" s="137"/>
-      <c r="D117" s="134"/>
-      <c r="E117" s="134"/>
-      <c r="F117" s="134"/>
-      <c r="G117" s="134"/>
-      <c r="H117" s="135"/>
+      <c r="C117" s="153"/>
+      <c r="D117" s="129"/>
+      <c r="E117" s="129"/>
+      <c r="F117" s="129"/>
+      <c r="G117" s="129"/>
+      <c r="H117" s="154"/>
     </row>
     <row r="118" spans="1:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="136"/>
-      <c r="B118" s="136"/>
-      <c r="C118" s="136"/>
-      <c r="D118" s="136"/>
-      <c r="E118" s="136"/>
-      <c r="F118" s="136"/>
-      <c r="G118" s="136"/>
-      <c r="H118" s="136"/>
+      <c r="A118" s="145"/>
+      <c r="B118" s="145"/>
+      <c r="C118" s="145"/>
+      <c r="D118" s="145"/>
+      <c r="E118" s="145"/>
+      <c r="F118" s="145"/>
+      <c r="G118" s="145"/>
+      <c r="H118" s="145"/>
     </row>
     <row r="119" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="25" t="s">
@@ -7179,96 +7331,116 @@
       <c r="B119" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C119" s="144"/>
-      <c r="D119" s="145"/>
-      <c r="E119" s="145"/>
-      <c r="F119" s="145"/>
-      <c r="G119" s="145"/>
-      <c r="H119" s="146"/>
+      <c r="C119" s="155"/>
+      <c r="D119" s="156"/>
+      <c r="E119" s="156"/>
+      <c r="F119" s="156"/>
+      <c r="G119" s="156"/>
+      <c r="H119" s="157"/>
     </row>
     <row r="120" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="27" t="s">
         <v>65</v>
       </c>
       <c r="B120" s="35"/>
-      <c r="C120" s="138"/>
-      <c r="D120" s="139"/>
-      <c r="E120" s="139"/>
-      <c r="F120" s="139"/>
-      <c r="G120" s="139"/>
-      <c r="H120" s="140"/>
+      <c r="C120" s="152"/>
+      <c r="D120" s="143"/>
+      <c r="E120" s="143"/>
+      <c r="F120" s="143"/>
+      <c r="G120" s="143"/>
+      <c r="H120" s="144"/>
     </row>
     <row r="121" spans="1:8" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A121" s="22" t="s">
         <v>257</v>
       </c>
       <c r="B121" s="35"/>
-      <c r="C121" s="147" t="s">
+      <c r="C121" s="211" t="s">
         <v>259</v>
       </c>
-      <c r="D121" s="148"/>
-      <c r="E121" s="148"/>
-      <c r="F121" s="148"/>
-      <c r="G121" s="148"/>
-      <c r="H121" s="149"/>
+      <c r="D121" s="212"/>
+      <c r="E121" s="212"/>
+      <c r="F121" s="212"/>
+      <c r="G121" s="212"/>
+      <c r="H121" s="213"/>
     </row>
     <row r="122" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A122" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B122" s="33"/>
-      <c r="C122" s="137"/>
-      <c r="D122" s="134"/>
-      <c r="E122" s="134"/>
-      <c r="F122" s="134"/>
-      <c r="G122" s="134"/>
-      <c r="H122" s="135"/>
+      <c r="C122" s="153"/>
+      <c r="D122" s="129"/>
+      <c r="E122" s="129"/>
+      <c r="F122" s="129"/>
+      <c r="G122" s="129"/>
+      <c r="H122" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="130">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="C49:H49"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="A57:H57"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="A67:H67"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="C122:H122"/>
+    <mergeCell ref="C105:H105"/>
+    <mergeCell ref="C106:H106"/>
+    <mergeCell ref="C110:H110"/>
+    <mergeCell ref="C111:H111"/>
+    <mergeCell ref="D107:H107"/>
+    <mergeCell ref="C119:H119"/>
+    <mergeCell ref="C113:H113"/>
+    <mergeCell ref="C120:H120"/>
+    <mergeCell ref="C114:H114"/>
+    <mergeCell ref="A118:H118"/>
+    <mergeCell ref="C117:H117"/>
+    <mergeCell ref="C121:H121"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="C71:H71"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C74:H74"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A78:H78"/>
+    <mergeCell ref="C79:H79"/>
+    <mergeCell ref="C80:H80"/>
+    <mergeCell ref="C61:H61"/>
+    <mergeCell ref="C62:H62"/>
+    <mergeCell ref="C63:H63"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C104:H104"/>
+    <mergeCell ref="C98:H98"/>
+    <mergeCell ref="A112:H112"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A103:H103"/>
+    <mergeCell ref="C102:H102"/>
+    <mergeCell ref="C100:F100"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="C95:H95"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C88:H88"/>
+    <mergeCell ref="C86:H86"/>
+    <mergeCell ref="C87:H87"/>
+    <mergeCell ref="C99:H99"/>
+    <mergeCell ref="C101:H101"/>
+    <mergeCell ref="D90:H90"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="C97:H97"/>
+    <mergeCell ref="C96:H96"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="C83:D83"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="C50:H50"/>
@@ -7293,69 +7465,49 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C104:H104"/>
-    <mergeCell ref="C98:H98"/>
-    <mergeCell ref="A112:H112"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A103:H103"/>
-    <mergeCell ref="C102:H102"/>
-    <mergeCell ref="C100:F100"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="C95:H95"/>
-    <mergeCell ref="C89:H89"/>
-    <mergeCell ref="C88:H88"/>
-    <mergeCell ref="C86:H86"/>
-    <mergeCell ref="C87:H87"/>
-    <mergeCell ref="C99:H99"/>
-    <mergeCell ref="C101:H101"/>
-    <mergeCell ref="D90:H90"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="C91:H91"/>
-    <mergeCell ref="C97:H97"/>
-    <mergeCell ref="C96:H96"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C75:H75"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="C74:H74"/>
-    <mergeCell ref="C60:H60"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A78:H78"/>
-    <mergeCell ref="C79:H79"/>
-    <mergeCell ref="C80:H80"/>
-    <mergeCell ref="C61:H61"/>
-    <mergeCell ref="C62:H62"/>
-    <mergeCell ref="C63:H63"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="A58:H58"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="A67:H67"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="C122:H122"/>
-    <mergeCell ref="C105:H105"/>
-    <mergeCell ref="C106:H106"/>
-    <mergeCell ref="C110:H110"/>
-    <mergeCell ref="C111:H111"/>
-    <mergeCell ref="D107:H107"/>
-    <mergeCell ref="C119:H119"/>
-    <mergeCell ref="C113:H113"/>
-    <mergeCell ref="C120:H120"/>
-    <mergeCell ref="C114:H114"/>
-    <mergeCell ref="A118:H118"/>
-    <mergeCell ref="C117:H117"/>
-    <mergeCell ref="C121:H121"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C4:H4"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -7589,19 +7741,19 @@
       </c>
       <c r="J2" s="124">
         <f>FS_Specs_IC_Powertrain!H10</f>
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="K2" s="124">
         <f>FS_Specs_IC_Powertrain!D10</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L2" s="124">
         <f>FS_Specs_IC_Powertrain!F10</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M2" t="str">
         <f>CONCATENATE(K2,"/",L2)</f>
-        <v>0/0</v>
+        <v>100/120</v>
       </c>
       <c r="N2" s="124" t="str">
         <f>FS_Specs_IC_Powertrain!C17</f>

</xml_diff>